<commit_message>
Add new data for attainment
</commit_message>
<xml_diff>
--- a/Duncan_Index/Duncan index by FINALAUG22.xlsx
+++ b/Duncan_Index/Duncan index by FINALAUG22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://impservihub-my.sharepoint.com/personal/nicholas_cassidy_improvementservice_org_uk/Documents/CPOP/Duncan_Index/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{9A9C2946-D7BA-4757-8564-DD044F70F428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{737A1855-C3E0-4852-9CCC-EDF75D04C43B}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{9A9C2946-D7BA-4757-8564-DD044F70F428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC1ED892-4958-4AEC-B76B-5E84C551427E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3150" yWindow="3255" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="2" r:id="rId1"/>
@@ -1127,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K385"/>
   <sheetViews>
-    <sheetView topLeftCell="A349" workbookViewId="0">
-      <selection activeCell="H385" sqref="H385"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,7 +1188,7 @@
         <v>0.37445802003318801</v>
       </c>
       <c r="H2">
-        <v>0.25193544948454899</v>
+        <v>0.25753066539302699</v>
       </c>
       <c r="I2">
         <v>-0.30856037331477998</v>
@@ -1223,7 +1223,7 @@
         <v>0.25307817167963598</v>
       </c>
       <c r="H3">
-        <v>0.114021398362024</v>
+        <v>0.12733232553677401</v>
       </c>
       <c r="I3">
         <v>-0.21990899156549301</v>
@@ -1258,7 +1258,7 @@
         <v>0.290494387962273</v>
       </c>
       <c r="H4">
-        <v>0.12828699944348701</v>
+        <v>0.13064065058602001</v>
       </c>
       <c r="I4">
         <v>-7.1796902001172405E-2</v>
@@ -1293,7 +1293,7 @@
         <v>0.18983994312836699</v>
       </c>
       <c r="H5">
-        <v>4.9165297504404598E-2</v>
+        <v>4.2883020047128198E-2</v>
       </c>
       <c r="I5">
         <v>-0.15790480150543301</v>
@@ -1363,7 +1363,7 @@
         <v>0.17305563410775099</v>
       </c>
       <c r="H7">
-        <v>0.13219969407409099</v>
+        <v>0.13584450200116499</v>
       </c>
       <c r="I7">
         <v>-0.117581439154486</v>
@@ -1398,7 +1398,7 @@
         <v>0.27564608470809299</v>
       </c>
       <c r="H8">
-        <v>0.248017187437725</v>
+        <v>0.24760404890066601</v>
       </c>
       <c r="I8">
         <v>-0.23124528843786701</v>
@@ -1433,7 +1433,7 @@
         <v>0.22342572566378699</v>
       </c>
       <c r="H9">
-        <v>0.18112121040034901</v>
+        <v>0.18634807053674499</v>
       </c>
       <c r="I9">
         <v>-0.23680838115450201</v>
@@ -1468,7 +1468,7 @@
         <v>0.34370767474310598</v>
       </c>
       <c r="H10">
-        <v>0.24884802586655599</v>
+        <v>0.25863047727851601</v>
       </c>
       <c r="I10">
         <v>-0.34477883779257901</v>
@@ -1538,7 +1538,7 @@
         <v>0.36895284602964201</v>
       </c>
       <c r="H12">
-        <v>0.30240236803322201</v>
+        <v>0.30553330048247901</v>
       </c>
       <c r="I12">
         <v>-0.28139818470011502</v>
@@ -1573,7 +1573,7 @@
         <v>0.43185738658648598</v>
       </c>
       <c r="H13">
-        <v>0.34120834822726198</v>
+        <v>0.34735801736722</v>
       </c>
       <c r="I13">
         <v>-0.32461989473547698</v>
@@ -1643,7 +1643,7 @@
         <v>0.199829963179395</v>
       </c>
       <c r="H15">
-        <v>0.19523966262957301</v>
+        <v>0.19997824236727799</v>
       </c>
       <c r="I15">
         <v>-0.16936913241044299</v>
@@ -1678,7 +1678,7 @@
         <v>0.29773550281905897</v>
       </c>
       <c r="H16">
-        <v>0.26910658142474397</v>
+        <v>0.28046042214734301</v>
       </c>
       <c r="I16">
         <v>-0.245455605191225</v>
@@ -1713,7 +1713,7 @@
         <v>0.230176990919055</v>
       </c>
       <c r="H17">
-        <v>0.162864949088245</v>
+        <v>0.16856378866379601</v>
       </c>
       <c r="I17">
         <v>-0.22670828620118799</v>
@@ -1748,7 +1748,7 @@
         <v>0.19438090875998501</v>
       </c>
       <c r="H18">
-        <v>0.12825262507440299</v>
+        <v>0.13333345198816099</v>
       </c>
       <c r="I18">
         <v>-0.15843775719279701</v>
@@ -1853,7 +1853,7 @@
         <v>7.9648634844096095E-2</v>
       </c>
       <c r="H21">
-        <v>4.5810053581665698E-2</v>
+        <v>4.8962422928168402E-2</v>
       </c>
       <c r="I21">
         <v>-9.0344305079058898E-2</v>
@@ -1888,7 +1888,7 @@
         <v>0.25328130489796102</v>
       </c>
       <c r="H22">
-        <v>0.20006802751882999</v>
+        <v>0.21290667066862701</v>
       </c>
       <c r="I22">
         <v>-0.22033053656457599</v>
@@ -1923,7 +1923,7 @@
         <v>0.19401769025655799</v>
       </c>
       <c r="H23">
-        <v>0.168114618407017</v>
+        <v>0.17288892219973601</v>
       </c>
       <c r="I23">
         <v>-0.122050552520392</v>
@@ -1958,7 +1958,7 @@
         <v>-2.4426564521902401E-2</v>
       </c>
       <c r="H24">
-        <v>-0.136285179566773</v>
+        <v>-4.6625454676756398E-2</v>
       </c>
       <c r="I24">
         <v>1.14579945844997E-2</v>
@@ -1993,7 +1993,7 @@
         <v>0.22528442178743899</v>
       </c>
       <c r="H25">
-        <v>0.114300054634375</v>
+        <v>0.11765729057133199</v>
       </c>
       <c r="I25">
         <v>-0.195722157014597</v>
@@ -2028,7 +2028,7 @@
         <v>0.32535498426022602</v>
       </c>
       <c r="H26">
-        <v>0.264950340397482</v>
+        <v>0.27005112111496599</v>
       </c>
       <c r="I26">
         <v>-0.32732453839550002</v>
@@ -2063,7 +2063,7 @@
         <v>0.177701141783974</v>
       </c>
       <c r="H27">
-        <v>0.140236545635434</v>
+        <v>0.145825220212913</v>
       </c>
       <c r="I27">
         <v>-7.2228060619771398E-2</v>
@@ -2098,7 +2098,7 @@
         <v>0.105634074505624</v>
       </c>
       <c r="H28">
-        <v>1.32449838617981E-2</v>
+        <v>3.5237482339829797E-2</v>
       </c>
       <c r="I28">
         <v>-4.8901904783378303E-2</v>
@@ -2133,7 +2133,7 @@
         <v>0.24128488913662599</v>
       </c>
       <c r="H29">
-        <v>0.21752169930996201</v>
+        <v>0.22733431446942001</v>
       </c>
       <c r="I29">
         <v>-0.217567237970481</v>
@@ -2168,7 +2168,7 @@
         <v>0.24117032836045399</v>
       </c>
       <c r="H30">
-        <v>0.21876987274561099</v>
+        <v>0.221893462292101</v>
       </c>
       <c r="I30">
         <v>-0.17861129154695399</v>
@@ -2203,7 +2203,7 @@
         <v>0.35106781400590997</v>
       </c>
       <c r="H31">
-        <v>0.31155276906923601</v>
+        <v>0.316028967438099</v>
       </c>
       <c r="I31">
         <v>-0.31258189885610799</v>
@@ -2238,7 +2238,7 @@
         <v>0.20335824517043699</v>
       </c>
       <c r="H32">
-        <v>0.173009498452904</v>
+        <v>0.18575018235951701</v>
       </c>
       <c r="I32">
         <v>-0.111689293541278</v>
@@ -2273,7 +2273,7 @@
         <v>0.234742903394102</v>
       </c>
       <c r="H33">
-        <v>0.22036070103159799</v>
+        <v>0.22577733473429401</v>
       </c>
       <c r="I33">
         <v>-0.17924835776325099</v>
@@ -2308,7 +2308,7 @@
         <v>0.35539978250277199</v>
       </c>
       <c r="H34">
-        <v>0.23125516634566901</v>
+        <v>0.24255258365889201</v>
       </c>
       <c r="I34">
         <v>-0.28822200205016402</v>
@@ -2343,7 +2343,7 @@
         <v>0.25735593998862399</v>
       </c>
       <c r="H35">
-        <v>0.124173277442246</v>
+        <v>0.13957667172339699</v>
       </c>
       <c r="I35">
         <v>-0.18625954896861399</v>
@@ -2378,7 +2378,7 @@
         <v>0.28537312863768499</v>
       </c>
       <c r="H36">
-        <v>0.160901776755352</v>
+        <v>0.16471238845698499</v>
       </c>
       <c r="I36">
         <v>-0.10855666391868</v>
@@ -2413,7 +2413,7 @@
         <v>0.203968390281064</v>
       </c>
       <c r="H37">
-        <v>6.68601049180442E-2</v>
+        <v>7.1757054084084601E-2</v>
       </c>
       <c r="I37">
         <v>-0.14280568038215799</v>
@@ -2483,7 +2483,7 @@
         <v>0.164711109281024</v>
       </c>
       <c r="H39">
-        <v>0.13980106659507599</v>
+        <v>0.14254853996838099</v>
       </c>
       <c r="I39">
         <v>-0.125949313338273</v>
@@ -2518,7 +2518,7 @@
         <v>0.29290428834416099</v>
       </c>
       <c r="H40">
-        <v>0.24615434508710099</v>
+        <v>0.24718331706493801</v>
       </c>
       <c r="I40">
         <v>-0.27689980755279597</v>
@@ -2553,7 +2553,7 @@
         <v>0.24431329822130199</v>
       </c>
       <c r="H41">
-        <v>0.20522142424943501</v>
+        <v>0.21884757193641699</v>
       </c>
       <c r="I41">
         <v>-0.21883799155319</v>
@@ -2588,7 +2588,7 @@
         <v>0.32974475036836798</v>
       </c>
       <c r="H42">
-        <v>0.25510896166910502</v>
+        <v>0.25716775832848199</v>
       </c>
       <c r="I42">
         <v>-0.304921467479016</v>
@@ -2623,7 +2623,7 @@
         <v>0.199202041427821</v>
       </c>
       <c r="H43">
-        <v>0.189225776611915</v>
+        <v>0.18981658895296999</v>
       </c>
       <c r="I43">
         <v>-0.17043262394949901</v>
@@ -2658,7 +2658,7 @@
         <v>0.403459885600428</v>
       </c>
       <c r="H44">
-        <v>0.32570012876232002</v>
+        <v>0.32955804256498</v>
       </c>
       <c r="I44">
         <v>-0.231421112853857</v>
@@ -2693,7 +2693,7 @@
         <v>0.40402271411220197</v>
       </c>
       <c r="H45">
-        <v>0.30986570183808498</v>
+        <v>0.31577612305210301</v>
       </c>
       <c r="I45">
         <v>-0.36650288467907899</v>
@@ -2763,7 +2763,7 @@
         <v>0.22104280760678199</v>
       </c>
       <c r="H47">
-        <v>0.21128514861634401</v>
+        <v>0.21640674035127999</v>
       </c>
       <c r="I47">
         <v>-0.14425385523376</v>
@@ -2798,7 +2798,7 @@
         <v>0.317830356393486</v>
       </c>
       <c r="H48">
-        <v>0.285053520986288</v>
+        <v>0.29455661653820198</v>
       </c>
       <c r="I48">
         <v>-0.29828496312167402</v>
@@ -2833,7 +2833,7 @@
         <v>0.22394610027357201</v>
       </c>
       <c r="H49">
-        <v>0.15034080817210299</v>
+        <v>0.15865667991775501</v>
       </c>
       <c r="I49">
         <v>-0.19508748723031699</v>
@@ -2868,7 +2868,7 @@
         <v>0.20088299788292799</v>
       </c>
       <c r="H50">
-        <v>0.13003145303310901</v>
+        <v>0.13628375640516299</v>
       </c>
       <c r="I50">
         <v>-0.160308864318431</v>
@@ -2903,7 +2903,7 @@
         <v>0.298355417016963</v>
       </c>
       <c r="H51">
-        <v>0.28510294108185302</v>
+        <v>0.294315680237623</v>
       </c>
       <c r="I51">
         <v>-0.26982621052049799</v>
@@ -2938,7 +2938,7 @@
         <v>0.226409354245308</v>
       </c>
       <c r="H52">
-        <v>0.21060437188526401</v>
+        <v>0.21023858456775299</v>
       </c>
       <c r="I52">
         <v>-0.21625466223547099</v>
@@ -2973,7 +2973,7 @@
         <v>7.9517113502468803E-2</v>
       </c>
       <c r="H53">
-        <v>5.8992285315878398E-2</v>
+        <v>6.0954145472786402E-2</v>
       </c>
       <c r="I53">
         <v>-0.11462532063905</v>
@@ -3008,7 +3008,7 @@
         <v>0.24715437995525</v>
       </c>
       <c r="H54">
-        <v>0.21033718738159199</v>
+        <v>0.220661287539031</v>
       </c>
       <c r="I54">
         <v>-0.202841823464393</v>
@@ -3043,7 +3043,7 @@
         <v>0.19780770644850401</v>
       </c>
       <c r="H55">
-        <v>0.16900150985606999</v>
+        <v>0.17232535438993701</v>
       </c>
       <c r="I55">
         <v>-0.136850477481094</v>
@@ -3113,7 +3113,7 @@
         <v>0.23875162207939701</v>
       </c>
       <c r="H57">
-        <v>0.15517129166271801</v>
+        <v>0.16183538941844799</v>
       </c>
       <c r="I57">
         <v>-0.21301180905995501</v>
@@ -3148,7 +3148,7 @@
         <v>0.32247326461307102</v>
       </c>
       <c r="H58">
-        <v>0.27217913582178399</v>
+        <v>0.27925975515351997</v>
       </c>
       <c r="I58">
         <v>-0.27314204363302302</v>
@@ -3183,7 +3183,7 @@
         <v>0.193818042629569</v>
       </c>
       <c r="H59">
-        <v>0.16365910781600199</v>
+        <v>0.16994272393137599</v>
       </c>
       <c r="I59">
         <v>-0.124556599189013</v>
@@ -3253,7 +3253,7 @@
         <v>0.22805983508493499</v>
       </c>
       <c r="H61">
-        <v>0.22061453001979101</v>
+        <v>0.22402294402950099</v>
       </c>
       <c r="I61">
         <v>-0.22828581846562701</v>
@@ -3288,7 +3288,7 @@
         <v>0.23835612715957699</v>
       </c>
       <c r="H62">
-        <v>0.222873207222584</v>
+        <v>0.225734858511565</v>
       </c>
       <c r="I62">
         <v>-0.16518967594383899</v>
@@ -3323,7 +3323,7 @@
         <v>0.34480561991728498</v>
       </c>
       <c r="H63">
-        <v>0.31109867946497399</v>
+        <v>0.31121092056175698</v>
       </c>
       <c r="I63">
         <v>-0.30690199890948999</v>
@@ -3358,7 +3358,7 @@
         <v>0.18490130433503499</v>
       </c>
       <c r="H64">
-        <v>0.161170416348065</v>
+        <v>0.16189497616369899</v>
       </c>
       <c r="I64">
         <v>-7.3976588654551798E-2</v>
@@ -3393,7 +3393,7 @@
         <v>0.21814615289762099</v>
       </c>
       <c r="H65">
-        <v>0.20469667701463801</v>
+        <v>0.20638745049308799</v>
       </c>
       <c r="I65">
         <v>-0.111587856745981</v>
@@ -3428,7 +3428,7 @@
         <v>0.35959972225140302</v>
       </c>
       <c r="H66">
-        <v>0.242552177843599</v>
+        <v>0.25166121509518602</v>
       </c>
       <c r="I66">
         <v>-0.283600979741294</v>
@@ -3463,7 +3463,7 @@
         <v>0.26760462835191801</v>
       </c>
       <c r="H67">
-        <v>0.13957009502262399</v>
+        <v>0.15178087977312801</v>
       </c>
       <c r="I67">
         <v>-0.202352619072595</v>
@@ -3498,7 +3498,7 @@
         <v>0.28778354774445902</v>
       </c>
       <c r="H68">
-        <v>0.16470858103792099</v>
+        <v>0.166416810038335</v>
       </c>
       <c r="I68">
         <v>-0.132834113920656</v>
@@ -3533,7 +3533,7 @@
         <v>0.20275143375288401</v>
       </c>
       <c r="H69">
-        <v>7.1753293130999707E-2</v>
+        <v>9.1160495247802203E-2</v>
       </c>
       <c r="I69">
         <v>-0.14743961812109099</v>
@@ -3603,7 +3603,7 @@
         <v>0.171774041783118</v>
       </c>
       <c r="H71">
-        <v>0.14254036665919401</v>
+        <v>0.14667350395825099</v>
       </c>
       <c r="I71">
         <v>-0.107059728491606</v>
@@ -3638,7 +3638,7 @@
         <v>0.31830435127317902</v>
       </c>
       <c r="H72">
-        <v>0.24718091604207101</v>
+        <v>0.25826158175472003</v>
       </c>
       <c r="I72">
         <v>-0.26015307018587602</v>
@@ -3673,7 +3673,7 @@
         <v>0.26395642452101797</v>
       </c>
       <c r="H73">
-        <v>0.21884441595238299</v>
+        <v>0.222764154308177</v>
       </c>
       <c r="I73">
         <v>-0.24895290804629999</v>
@@ -3708,7 +3708,7 @@
         <v>0.33544743520749298</v>
       </c>
       <c r="H74">
-        <v>0.25717531554075101</v>
+        <v>0.26749271612879399</v>
       </c>
       <c r="I74">
         <v>-0.288657254727966</v>
@@ -3778,7 +3778,7 @@
         <v>0.40531313184846302</v>
       </c>
       <c r="H76">
-        <v>0.32956074551516101</v>
+        <v>0.337323143588105</v>
       </c>
       <c r="I76">
         <v>-0.26416738883955099</v>
@@ -3813,7 +3813,7 @@
         <v>0.41263103439279503</v>
       </c>
       <c r="H77">
-        <v>0.31577570882878803</v>
+        <v>0.323594579401906</v>
       </c>
       <c r="I77">
         <v>-0.34348118193044302</v>
@@ -3848,7 +3848,7 @@
         <v>2.1776148709177899E-2</v>
       </c>
       <c r="H78">
-        <v>-4.3770354748443402E-2</v>
+        <v>-4.869922438911E-2</v>
       </c>
       <c r="I78">
         <v>-9.5259310119382191E-3</v>
@@ -3883,7 +3883,7 @@
         <v>0.24071216621376801</v>
       </c>
       <c r="H79">
-        <v>0.21640734317672999</v>
+        <v>0.222246548416006</v>
       </c>
       <c r="I79">
         <v>-0.180035000301038</v>
@@ -3918,7 +3918,7 @@
         <v>0.32630777736734701</v>
       </c>
       <c r="H80">
-        <v>0.29455408976205899</v>
+        <v>0.30483678133202802</v>
       </c>
       <c r="I80">
         <v>-0.328301632647445</v>
@@ -3953,7 +3953,7 @@
         <v>0.23471042374010401</v>
       </c>
       <c r="H81">
-        <v>0.158655878380145</v>
+        <v>0.165593677872899</v>
       </c>
       <c r="I81">
         <v>-0.19462100788098999</v>
@@ -3988,7 +3988,7 @@
         <v>0.20931530592057601</v>
       </c>
       <c r="H82">
-        <v>0.13628211484875399</v>
+        <v>0.144214059430361</v>
       </c>
       <c r="I82">
         <v>-0.175957182124719</v>
@@ -4058,7 +4058,7 @@
         <v>0.23072870191466199</v>
       </c>
       <c r="H84">
-        <v>0.21024530391961599</v>
+        <v>0.210164369660234</v>
       </c>
       <c r="I84">
         <v>-0.12213353990803</v>
@@ -4093,7 +4093,7 @@
         <v>8.61305072552732E-2</v>
       </c>
       <c r="H85">
-        <v>6.09502064660443E-2</v>
+        <v>6.4698532748412405E-2</v>
       </c>
       <c r="I85">
         <v>-0.120978936719826</v>
@@ -4128,7 +4128,7 @@
         <v>0.26056450310127699</v>
       </c>
       <c r="H86">
-        <v>0.22065631592340501</v>
+        <v>0.240637115921494</v>
       </c>
       <c r="I86">
         <v>-0.19481807484907601</v>
@@ -4163,7 +4163,7 @@
         <v>0.203351354332092</v>
       </c>
       <c r="H87">
-        <v>0.172327365434846</v>
+        <v>0.17645399272250401</v>
       </c>
       <c r="I87">
         <v>-0.15508661249696901</v>
@@ -4233,7 +4233,7 @@
         <v>0.25425545475647499</v>
       </c>
       <c r="H89">
-        <v>0.16183855342883099</v>
+        <v>0.18197645125960099</v>
       </c>
       <c r="I89">
         <v>-0.19000826243990199</v>
@@ -4268,7 +4268,7 @@
         <v>0.32918969922126401</v>
       </c>
       <c r="H90">
-        <v>0.27925717717634402</v>
+        <v>0.28923976654384698</v>
       </c>
       <c r="I90">
         <v>-0.236199538365469</v>
@@ -4303,7 +4303,7 @@
         <v>0.205752871878742</v>
       </c>
       <c r="H91">
-        <v>0.16994652116378201</v>
+        <v>0.17339995708459799</v>
       </c>
       <c r="I91">
         <v>-8.5503911152835996E-2</v>
@@ -4338,7 +4338,7 @@
         <v>9.6901606719111702E-2</v>
       </c>
       <c r="H92">
-        <v>-5.3600904362882695E-4</v>
+        <v>-1.06681279083629E-2</v>
       </c>
       <c r="I92">
         <v>1.46719886146851E-2</v>
@@ -4373,7 +4373,7 @@
         <v>0.22980688993603601</v>
       </c>
       <c r="H93">
-        <v>0.22402318937750501</v>
+        <v>0.23279843696243299</v>
       </c>
       <c r="I93">
         <v>-0.20678998377355501</v>
@@ -4408,7 +4408,7 @@
         <v>0.24707503062044001</v>
       </c>
       <c r="H94">
-        <v>0.22573198183798099</v>
+        <v>0.23179690194003699</v>
       </c>
       <c r="I94">
         <v>-0.13349892563211799</v>
@@ -4478,7 +4478,7 @@
         <v>0.190215351268611</v>
       </c>
       <c r="H96">
-        <v>0.16189422729136099</v>
+        <v>0.16467792109795501</v>
       </c>
       <c r="I96">
         <v>-0.13128417139527801</v>
@@ -4513,7 +4513,7 @@
         <v>0.22335829123539999</v>
       </c>
       <c r="H97">
-        <v>0.20638796132176301</v>
+        <v>0.20935105374128299</v>
       </c>
       <c r="I97">
         <v>-0.12841165124323201</v>
@@ -4548,7 +4548,7 @@
         <v>0.35862753012020598</v>
       </c>
       <c r="H98">
-        <v>0.25166121509518602</v>
+        <v>0.25967410488441101</v>
       </c>
       <c r="I98">
         <v>-0.29883078301310401</v>
@@ -4583,7 +4583,7 @@
         <v>0.27388670904286999</v>
       </c>
       <c r="H99">
-        <v>0.15178087977312801</v>
+        <v>0.16610242876595599</v>
       </c>
       <c r="I99">
         <v>-0.161142242329124</v>
@@ -4618,7 +4618,7 @@
         <v>0.296322299541254</v>
       </c>
       <c r="H100">
-        <v>0.166416810038335</v>
+        <v>0.19612948422843399</v>
       </c>
       <c r="I100">
         <v>-0.104468612726622</v>
@@ -4653,7 +4653,7 @@
         <v>0.21028648687377299</v>
       </c>
       <c r="H101">
-        <v>9.1160495247802203E-2</v>
+        <v>9.4199658855860194E-2</v>
       </c>
       <c r="I101">
         <v>-0.19910538162594699</v>
@@ -4688,7 +4688,7 @@
         <v>0.16876914819456901</v>
       </c>
       <c r="H102">
-        <v>0.23117964120418499</v>
+        <v>0.23209915984462601</v>
       </c>
       <c r="I102">
         <v>-6.8736478475304202E-2</v>
@@ -4723,7 +4723,7 @@
         <v>0.17967326277856099</v>
       </c>
       <c r="H103">
-        <v>0.14667350395825099</v>
+        <v>0.154726580542805</v>
       </c>
       <c r="I103">
         <v>-0.14697807056495699</v>
@@ -4758,7 +4758,7 @@
         <v>0.32720096642115898</v>
       </c>
       <c r="H104">
-        <v>0.25826158175472003</v>
+        <v>0.26296694689990702</v>
       </c>
       <c r="I104">
         <v>-0.217513508351979</v>
@@ -4793,7 +4793,7 @@
         <v>0.26954129888223699</v>
       </c>
       <c r="H105">
-        <v>0.222764154308177</v>
+        <v>0.23097215601896301</v>
       </c>
       <c r="I105">
         <v>-0.204331222417407</v>
@@ -4828,7 +4828,7 @@
         <v>0.33771364555379302</v>
       </c>
       <c r="H106">
-        <v>0.26749271612879399</v>
+        <v>0.27928287989694001</v>
       </c>
       <c r="I106">
         <v>-0.26486858073108399</v>
@@ -4863,7 +4863,7 @@
         <v>0.20106060480598101</v>
       </c>
       <c r="H107">
-        <v>0.189816201933283</v>
+        <v>0.189922204773495</v>
       </c>
       <c r="I107">
         <v>-0.15834060005492501</v>
@@ -4898,7 +4898,7 @@
         <v>0.40615394876284999</v>
       </c>
       <c r="H108">
-        <v>0.337323143588105</v>
+        <v>0.34249242721103401</v>
       </c>
       <c r="I108">
         <v>-0.32790006183492298</v>
@@ -4933,7 +4933,7 @@
         <v>0.419708395006687</v>
       </c>
       <c r="H109">
-        <v>0.323594579401906</v>
+        <v>0.33030679694474002</v>
       </c>
       <c r="I109">
         <v>-0.34647570318100301</v>
@@ -4968,7 +4968,7 @@
         <v>2.64172734705546E-2</v>
       </c>
       <c r="H110">
-        <v>-4.869922438911E-2</v>
+        <v>-5.0122141468833099E-2</v>
       </c>
       <c r="I110">
         <v>-8.5054524906347196E-4</v>
@@ -5003,7 +5003,7 @@
         <v>0.25732955658761902</v>
       </c>
       <c r="H111">
-        <v>0.222246548416006</v>
+        <v>0.23258102643422701</v>
       </c>
       <c r="I111">
         <v>-0.202407155839992</v>
@@ -5038,7 +5038,7 @@
         <v>0.338650873382846</v>
       </c>
       <c r="H112">
-        <v>0.30483678133202802</v>
+        <v>0.31444472699960402</v>
       </c>
       <c r="I112">
         <v>-0.332473033180825</v>
@@ -5073,7 +5073,7 @@
         <v>0.25278610643981397</v>
       </c>
       <c r="H113">
-        <v>0.165593677872899</v>
+        <v>0.17272609110565201</v>
       </c>
       <c r="I113">
         <v>-0.20842831675974999</v>
@@ -5108,7 +5108,7 @@
         <v>0.22736091863036001</v>
       </c>
       <c r="H114">
-        <v>0.144214059430361</v>
+        <v>0.15081628295951399</v>
       </c>
       <c r="I114">
         <v>-0.177700714694083</v>
@@ -5143,7 +5143,7 @@
         <v>0.31904258490952903</v>
       </c>
       <c r="H115">
-        <v>0.29432272404037801</v>
+        <v>0.29496579588585398</v>
       </c>
       <c r="I115">
         <v>-0.31216104317457299</v>
@@ -5178,7 +5178,7 @@
         <v>0.230168339705522</v>
       </c>
       <c r="H116">
-        <v>0.210164369660234</v>
+        <v>0.20891916459224699</v>
       </c>
       <c r="I116">
         <v>-0.190125339562214</v>
@@ -5213,7 +5213,7 @@
         <v>9.9593955933221096E-2</v>
       </c>
       <c r="H117">
-        <v>6.4698532748412405E-2</v>
+        <v>6.8765215095464099E-2</v>
       </c>
       <c r="I117">
         <v>-9.7381757945997904E-2</v>
@@ -5248,7 +5248,7 @@
         <v>0.262164587375526</v>
       </c>
       <c r="H118">
-        <v>0.240637115921494</v>
+        <v>0.25369801979745599</v>
       </c>
       <c r="I118">
         <v>-0.19402949377125001</v>
@@ -5283,7 +5283,7 @@
         <v>0.20808259033194099</v>
       </c>
       <c r="H119">
-        <v>0.17645399272250401</v>
+        <v>0.18087975008370799</v>
       </c>
       <c r="I119">
         <v>-0.179278244423873</v>
@@ -5318,7 +5318,7 @@
         <v>7.2468393588040095E-2</v>
       </c>
       <c r="H120">
-        <v>-1.09590058026467E-2</v>
+        <v>5.1632405290236204E-3</v>
       </c>
       <c r="I120">
         <v>-0.14807291542671999</v>
@@ -5353,7 +5353,7 @@
         <v>0.25568068336696498</v>
       </c>
       <c r="H121">
-        <v>0.18197645125960099</v>
+        <v>0.19179159541926999</v>
       </c>
       <c r="I121">
         <v>-0.20550709543510401</v>
@@ -5388,7 +5388,7 @@
         <v>0.33339830753319999</v>
       </c>
       <c r="H122">
-        <v>0.28923976654384698</v>
+        <v>0.303875288694886</v>
       </c>
       <c r="I122">
         <v>-0.28468648277570602</v>
@@ -5423,7 +5423,7 @@
         <v>0.223124018960531</v>
       </c>
       <c r="H123">
-        <v>0.17339995708459799</v>
+        <v>0.180480998477172</v>
       </c>
       <c r="I123">
         <v>-0.13772000522576999</v>
@@ -5493,7 +5493,7 @@
         <v>0.23254131909953199</v>
       </c>
       <c r="H125">
-        <v>0.23279843696243299</v>
+        <v>0.243630838563309</v>
       </c>
       <c r="I125">
         <v>-0.20920687422341899</v>
@@ -5528,7 +5528,7 @@
         <v>0.25177075341000699</v>
       </c>
       <c r="H126">
-        <v>0.23179690194003699</v>
+        <v>0.236813496064084</v>
       </c>
       <c r="I126">
         <v>-0.117143048618033</v>
@@ -5563,7 +5563,7 @@
         <v>0.35284681703760501</v>
       </c>
       <c r="H127">
-        <v>0.31121865348188199</v>
+        <v>0.31237057519773298</v>
       </c>
       <c r="I127">
         <v>-0.30119074275083402</v>
@@ -5598,7 +5598,7 @@
         <v>0.19505938105666601</v>
       </c>
       <c r="H128">
-        <v>0.16467792109795501</v>
+        <v>0.165539178525207</v>
       </c>
       <c r="I128">
         <v>-0.11570890162056401</v>
@@ -5633,7 +5633,7 @@
         <v>0.22871572617374999</v>
       </c>
       <c r="H129">
-        <v>0.20935105374128299</v>
+        <v>0.21157261356901799</v>
       </c>
       <c r="I129">
         <v>-0.14606980634648001</v>
@@ -5668,7 +5668,7 @@
         <v>0.35348469607017202</v>
       </c>
       <c r="H130">
-        <v>0.272875252973655</v>
+        <v>0.279796855831691</v>
       </c>
       <c r="I130">
         <v>-0.33436911024501398</v>
@@ -5703,7 +5703,7 @@
         <v>0.28400289640959597</v>
       </c>
       <c r="H131">
-        <v>0.18780805908515999</v>
+        <v>0.20420990429834199</v>
       </c>
       <c r="I131">
         <v>-0.20207807958922799</v>
@@ -5738,7 +5738,7 @@
         <v>0.28245496678784199</v>
       </c>
       <c r="H132">
-        <v>0.17180830630459301</v>
+        <v>0.18480148195075499</v>
       </c>
       <c r="I132">
         <v>-0.15984978080875401</v>
@@ -5773,7 +5773,7 @@
         <v>0.17618173665837999</v>
       </c>
       <c r="H133">
-        <v>9.8726881986058501E-2</v>
+        <v>0.10864352829238499</v>
       </c>
       <c r="I133">
         <v>-0.191333946220173</v>
@@ -5843,7 +5843,7 @@
         <v>0.20056015536246</v>
       </c>
       <c r="H135">
-        <v>0.171604535926212</v>
+        <v>0.174919672076049</v>
       </c>
       <c r="I135">
         <v>-0.151670655213172</v>
@@ -5878,7 +5878,7 @@
         <v>0.32692660160093601</v>
       </c>
       <c r="H136">
-        <v>0.28167023907666999</v>
+        <v>0.290214460947265</v>
       </c>
       <c r="I136">
         <v>-0.19263349998670301</v>
@@ -5913,7 +5913,7 @@
         <v>0.25696238521959802</v>
       </c>
       <c r="H137">
-        <v>0.21062280734844699</v>
+        <v>0.23333064833314199</v>
       </c>
       <c r="I137">
         <v>-0.23026057894872101</v>
@@ -5948,7 +5948,7 @@
         <v>0.33439568200485997</v>
       </c>
       <c r="H138">
-        <v>0.27941382533718501</v>
+        <v>0.28123184460428902</v>
       </c>
       <c r="I138">
         <v>-0.33409605430775402</v>
@@ -5983,7 +5983,7 @@
         <v>0.23135925763118301</v>
       </c>
       <c r="H139">
-        <v>0.230726003134158</v>
+        <v>0.23339192330643499</v>
       </c>
       <c r="I139">
         <v>-0.19587722778303299</v>
@@ -6018,7 +6018,7 @@
         <v>0.39835885123280101</v>
       </c>
       <c r="H140">
-        <v>0.350371392513049</v>
+        <v>0.35603829223997302</v>
       </c>
       <c r="I140">
         <v>-0.34548108474158901</v>
@@ -6053,7 +6053,7 @@
         <v>0.44670473908462999</v>
       </c>
       <c r="H141">
-        <v>0.36491681063783699</v>
+        <v>0.369385921062928</v>
       </c>
       <c r="I141">
         <v>-0.38474481666762</v>
@@ -6088,7 +6088,7 @@
         <v>-1.7009990851533101E-3</v>
       </c>
       <c r="H142">
-        <v>-6.6433456218693898E-2</v>
+        <v>-5.5755292071629999E-2</v>
       </c>
       <c r="I142">
         <v>-3.8738199835146599E-2</v>
@@ -6123,7 +6123,7 @@
         <v>0.238460756476188</v>
       </c>
       <c r="H143">
-        <v>0.23623015303305001</v>
+        <v>0.24091797231137099</v>
       </c>
       <c r="I143">
         <v>-0.210078832276377</v>
@@ -6158,7 +6158,7 @@
         <v>0.331490490254573</v>
       </c>
       <c r="H144">
-        <v>0.30205352755888998</v>
+        <v>0.309025407408065</v>
       </c>
       <c r="I144">
         <v>-0.27608994798512798</v>
@@ -6193,7 +6193,7 @@
         <v>0.26049082119147499</v>
       </c>
       <c r="H145">
-        <v>0.19316389834850201</v>
+        <v>0.20260648485362501</v>
       </c>
       <c r="I145">
         <v>-0.22334212361950301</v>
@@ -6228,7 +6228,7 @@
         <v>0.234560164622511</v>
       </c>
       <c r="H146">
-        <v>0.16694261573737601</v>
+        <v>0.171962862950021</v>
       </c>
       <c r="I146">
         <v>-0.18582173671111901</v>
@@ -6263,7 +6263,7 @@
         <v>0.32443756050751399</v>
       </c>
       <c r="H147">
-        <v>0.29787733024025398</v>
+        <v>0.29971266501335497</v>
       </c>
       <c r="I147">
         <v>-0.31393760581805202</v>
@@ -6298,7 +6298,7 @@
         <v>0.26738509484305101</v>
       </c>
       <c r="H148">
-        <v>0.218829788286281</v>
+        <v>0.222062741812557</v>
       </c>
       <c r="I148">
         <v>-0.19845445803913001</v>
@@ -6333,7 +6333,7 @@
         <v>0.139512263244818</v>
       </c>
       <c r="H149">
-        <v>6.2653684524277303E-2</v>
+        <v>7.5735247498995406E-2</v>
       </c>
       <c r="I149">
         <v>-9.6531497427546006E-2</v>
@@ -6368,7 +6368,7 @@
         <v>0.27102627798132101</v>
       </c>
       <c r="H150">
-        <v>0.23777333197196199</v>
+        <v>0.253222884296884</v>
       </c>
       <c r="I150">
         <v>-0.23814133116439301</v>
@@ -6403,7 +6403,7 @@
         <v>0.21110738376645699</v>
       </c>
       <c r="H151">
-        <v>0.19038899154313399</v>
+        <v>0.194997075716596</v>
       </c>
       <c r="I151">
         <v>-0.159193691172302</v>
@@ -6438,7 +6438,7 @@
         <v>0.103421935501433</v>
       </c>
       <c r="H152">
-        <v>-4.0514055896942996E-3</v>
+        <v>4.4088765490067898E-2</v>
       </c>
       <c r="I152">
         <v>-0.18694376960714201</v>
@@ -6473,7 +6473,7 @@
         <v>0.28098719783589798</v>
       </c>
       <c r="H153">
-        <v>0.18166572258585301</v>
+        <v>0.20918444206370501</v>
       </c>
       <c r="I153">
         <v>-0.20854680534175801</v>
@@ -6508,7 +6508,7 @@
         <v>0.34125321745544401</v>
       </c>
       <c r="H154">
-        <v>0.31964089365010701</v>
+        <v>0.327180615313518</v>
       </c>
       <c r="I154">
         <v>-0.28031985912063301</v>
@@ -6543,7 +6543,7 @@
         <v>0.226829982414637</v>
       </c>
       <c r="H155">
-        <v>0.19801789396416</v>
+        <v>0.211236620735471</v>
       </c>
       <c r="I155">
         <v>-0.14826528188949001</v>
@@ -6613,7 +6613,7 @@
         <v>0.28160554081144401</v>
       </c>
       <c r="H157">
-        <v>0.28465244510571402</v>
+        <v>0.28929355111716298</v>
       </c>
       <c r="I157">
         <v>-0.245751314742882</v>
@@ -6648,7 +6648,7 @@
         <v>0.24982072025052601</v>
       </c>
       <c r="H158">
-        <v>0.22794736850735101</v>
+        <v>0.23262868028981401</v>
       </c>
       <c r="I158">
         <v>-0.13806951302714399</v>
@@ -6683,7 +6683,7 @@
         <v>0.35168687718574898</v>
       </c>
       <c r="H159">
-        <v>0.31480543935126098</v>
+        <v>0.31539834337524802</v>
       </c>
       <c r="I159">
         <v>-0.30794612401881599</v>
@@ -6718,7 +6718,7 @@
         <v>0.217204291848867</v>
       </c>
       <c r="H160">
-        <v>0.180460752406298</v>
+        <v>0.185269040202339</v>
       </c>
       <c r="I160">
         <v>-0.123360111105436</v>
@@ -6753,7 +6753,7 @@
         <v>0.25819063051471097</v>
       </c>
       <c r="H161">
-        <v>0.232796039478945</v>
+        <v>0.238495876837236</v>
       </c>
       <c r="I161">
         <v>-0.177675023223793</v>
@@ -6788,7 +6788,7 @@
         <v>0.32822436390182802</v>
       </c>
       <c r="H162">
-        <v>0.279796855831691</v>
+        <v>0.288693240628625</v>
       </c>
       <c r="I162">
         <v>-0.31677916971947401</v>
@@ -6823,7 +6823,7 @@
         <v>0.28689900578965299</v>
       </c>
       <c r="H163">
-        <v>0.20420990429834199</v>
+        <v>0.222031133769441</v>
       </c>
       <c r="I163">
         <v>-0.19068897491019099</v>
@@ -6858,7 +6858,7 @@
         <v>0.271237681584449</v>
       </c>
       <c r="H164">
-        <v>0.18480148195075499</v>
+        <v>0.210083912843396</v>
       </c>
       <c r="I164">
         <v>-0.208067868725125</v>
@@ -6893,7 +6893,7 @@
         <v>0.196710693755758</v>
       </c>
       <c r="H165">
-        <v>0.10864352829238499</v>
+        <v>0.12324033308250799</v>
       </c>
       <c r="I165">
         <v>-0.20060494134145601</v>
@@ -6928,7 +6928,7 @@
         <v>0.239774896806872</v>
       </c>
       <c r="H166">
-        <v>0.23588558608384799</v>
+        <v>0.23643059578603301</v>
       </c>
       <c r="I166">
         <v>-0.16264346266455401</v>
@@ -6963,7 +6963,7 @@
         <v>0.20290354529885801</v>
       </c>
       <c r="H167">
-        <v>0.174919672076049</v>
+        <v>0.178747603817907</v>
       </c>
       <c r="I167">
         <v>-0.178853512826704</v>
@@ -6998,7 +6998,7 @@
         <v>0.324280097332661</v>
       </c>
       <c r="H168">
-        <v>0.290214460947265</v>
+        <v>0.293445446506928</v>
       </c>
       <c r="I168">
         <v>-0.21268378852750999</v>
@@ -7033,7 +7033,7 @@
         <v>0.24945557495774101</v>
       </c>
       <c r="H169">
-        <v>0.23333064833314199</v>
+        <v>0.24271629355461299</v>
       </c>
       <c r="I169">
         <v>-0.22062428083664201</v>
@@ -7068,7 +7068,7 @@
         <v>0.32459175491703501</v>
       </c>
       <c r="H170">
-        <v>0.28123184460428902</v>
+        <v>0.295990995084571</v>
       </c>
       <c r="I170">
         <v>-0.31729073912633199</v>
@@ -7103,7 +7103,7 @@
         <v>0.24179131964844</v>
       </c>
       <c r="H171">
-        <v>0.23339192330643499</v>
+        <v>0.230758800138467</v>
       </c>
       <c r="I171">
         <v>-0.21605176849274901</v>
@@ -7138,7 +7138,7 @@
         <v>0.41079267751056597</v>
       </c>
       <c r="H172">
-        <v>0.35603829223997302</v>
+        <v>0.36266265627130001</v>
       </c>
       <c r="I172">
         <v>-0.36708323769068102</v>
@@ -7173,7 +7173,7 @@
         <v>0.44874446917925298</v>
       </c>
       <c r="H173">
-        <v>0.369385921062928</v>
+        <v>0.37570599148168099</v>
       </c>
       <c r="I173">
         <v>-0.40138285336965801</v>
@@ -7208,7 +7208,7 @@
         <v>3.0271464932382801E-2</v>
       </c>
       <c r="H174">
-        <v>-5.5755292071629999E-2</v>
+        <v>-6.4445503211021396E-2</v>
       </c>
       <c r="I174">
         <v>1.7482595266347101E-2</v>
@@ -7243,7 +7243,7 @@
         <v>0.247589515257507</v>
       </c>
       <c r="H175">
-        <v>0.24091797231137099</v>
+        <v>0.25024326553560899</v>
       </c>
       <c r="I175">
         <v>-0.200265389432213</v>
@@ -7278,7 +7278,7 @@
         <v>0.337473254157374</v>
       </c>
       <c r="H176">
-        <v>0.309025407408065</v>
+        <v>0.31795994448697201</v>
       </c>
       <c r="I176">
         <v>-0.28813074135696598</v>
@@ -7313,7 +7313,7 @@
         <v>0.28057428401798001</v>
       </c>
       <c r="H177">
-        <v>0.20260648485362501</v>
+        <v>0.210713452126079</v>
       </c>
       <c r="I177">
         <v>-0.201159861314224</v>
@@ -7348,7 +7348,7 @@
         <v>0.25199231869850902</v>
       </c>
       <c r="H178">
-        <v>0.171962862950021</v>
+        <v>0.180349699891799</v>
       </c>
       <c r="I178">
         <v>-0.211926201443248</v>
@@ -7383,7 +7383,7 @@
         <v>0.32080638066594902</v>
       </c>
       <c r="H179">
-        <v>0.29971266501335497</v>
+        <v>0.301832704743072</v>
       </c>
       <c r="I179">
         <v>-0.26163910537257401</v>
@@ -7418,7 +7418,7 @@
         <v>0.25360560517263903</v>
       </c>
       <c r="H180">
-        <v>0.222062741812557</v>
+        <v>0.22978715014787099</v>
       </c>
       <c r="I180">
         <v>-0.16390511925521001</v>
@@ -7453,7 +7453,7 @@
         <v>0.106404018831563</v>
       </c>
       <c r="H181">
-        <v>7.5735247498995406E-2</v>
+        <v>9.28291073282317E-2</v>
       </c>
       <c r="I181">
         <v>-6.9974629541636801E-2</v>
@@ -7488,7 +7488,7 @@
         <v>0.27635261178019699</v>
       </c>
       <c r="H182">
-        <v>0.253222884296884</v>
+        <v>0.26695020551718701</v>
       </c>
       <c r="I182">
         <v>-0.198450210562614</v>
@@ -7523,7 +7523,7 @@
         <v>0.203132397937903</v>
       </c>
       <c r="H183">
-        <v>0.194997075716596</v>
+        <v>0.19895881810891999</v>
       </c>
       <c r="I183">
         <v>-0.16118854399524801</v>
@@ -7593,7 +7593,7 @@
         <v>0.279554385925048</v>
       </c>
       <c r="H185">
-        <v>0.20918444206370501</v>
+        <v>0.22089121268454401</v>
       </c>
       <c r="I185">
         <v>-0.23154761186019401</v>
@@ -7628,7 +7628,7 @@
         <v>0.33558544184313999</v>
       </c>
       <c r="H186">
-        <v>0.327180615313518</v>
+        <v>0.33289396771472102</v>
       </c>
       <c r="I186">
         <v>-0.31462198557550503</v>
@@ -7663,7 +7663,7 @@
         <v>0.22913725544201199</v>
       </c>
       <c r="H187">
-        <v>0.211236620735471</v>
+        <v>0.213061405645256</v>
       </c>
       <c r="I187">
         <v>-0.170858273872215</v>
@@ -7733,7 +7733,7 @@
         <v>0.26884614955591801</v>
       </c>
       <c r="H189">
-        <v>0.28929355111716298</v>
+        <v>0.29014260316087498</v>
       </c>
       <c r="I189">
         <v>-0.27252697199991699</v>
@@ -7768,7 +7768,7 @@
         <v>0.252721247169237</v>
       </c>
       <c r="H190">
-        <v>0.23262868028981401</v>
+        <v>0.23846305120319</v>
       </c>
       <c r="I190">
         <v>-0.149904421106797</v>
@@ -7803,7 +7803,7 @@
         <v>0.345916008758135</v>
       </c>
       <c r="H191">
-        <v>0.31539834337524802</v>
+        <v>0.31797267626356901</v>
       </c>
       <c r="I191">
         <v>-0.307851515082677</v>
@@ -7838,7 +7838,7 @@
         <v>0.22243504026541899</v>
       </c>
       <c r="H192">
-        <v>0.185269040202339</v>
+        <v>0.188437142288848</v>
       </c>
       <c r="I192">
         <v>-0.127240586107084</v>
@@ -7873,7 +7873,7 @@
         <v>0.249194247113184</v>
       </c>
       <c r="H193">
-        <v>0.238495876837236</v>
+        <v>0.243959330553492</v>
       </c>
       <c r="I193">
         <v>-0.19353487477189699</v>
@@ -7908,7 +7908,7 @@
         <v>0.33227242697690001</v>
       </c>
       <c r="H194">
-        <v>0.288693240628625</v>
+        <v>0.30371995660623302</v>
       </c>
       <c r="I194">
         <v>-0.31437279082471098</v>
@@ -7943,7 +7943,7 @@
         <v>0.29962180547795503</v>
       </c>
       <c r="H195">
-        <v>0.222031133769441</v>
+        <v>0.23764270124214101</v>
       </c>
       <c r="I195">
         <v>-0.21872636224535599</v>
@@ -7978,7 +7978,7 @@
         <v>0.27298020930143402</v>
       </c>
       <c r="H196">
-        <v>0.210083912843396</v>
+        <v>0.225488600947962</v>
       </c>
       <c r="I196">
         <v>-0.16635718461229099</v>
@@ -8013,7 +8013,7 @@
         <v>0.16550519734902</v>
       </c>
       <c r="H197">
-        <v>0.12324033308250799</v>
+        <v>0.11998419568173101</v>
       </c>
       <c r="I197">
         <v>-0.18227256778819101</v>
@@ -8083,7 +8083,7 @@
         <v>0.21350004960005201</v>
       </c>
       <c r="H199">
-        <v>0.178747603817907</v>
+        <v>0.179325959440677</v>
       </c>
       <c r="I199">
         <v>-0.16277682327161699</v>
@@ -8118,7 +8118,7 @@
         <v>0.31660920006382498</v>
       </c>
       <c r="H200">
-        <v>0.293445446506928</v>
+        <v>0.30069367803100799</v>
       </c>
       <c r="I200">
         <v>-0.22738705355955699</v>
@@ -8153,7 +8153,7 @@
         <v>0.25883018852526102</v>
       </c>
       <c r="H201">
-        <v>0.24271629355461299</v>
+        <v>0.25533378869606199</v>
       </c>
       <c r="I201">
         <v>-0.22075011639584499</v>
@@ -8188,7 +8188,7 @@
         <v>0.30929094500811899</v>
       </c>
       <c r="H202">
-        <v>0.295990995084571</v>
+        <v>0.31304944031251097</v>
       </c>
       <c r="I202">
         <v>-0.27015781723487903</v>
@@ -8223,7 +8223,7 @@
         <v>0.22867219245017401</v>
       </c>
       <c r="H203">
-        <v>0.230758800138467</v>
+        <v>0.23001612103494101</v>
       </c>
       <c r="I203">
         <v>-0.20321815858273801</v>
@@ -8258,7 +8258,7 @@
         <v>0.40901271277741902</v>
       </c>
       <c r="H204">
-        <v>0.36266265627130001</v>
+        <v>0.365617631668052</v>
       </c>
       <c r="I204">
         <v>-0.340309750273736</v>
@@ -8293,7 +8293,7 @@
         <v>0.44750740952356</v>
       </c>
       <c r="H205">
-        <v>0.37570599148168099</v>
+        <v>0.38362973718555099</v>
       </c>
       <c r="I205">
         <v>-0.374907355608464</v>
@@ -8363,7 +8363,7 @@
         <v>0.249144524983544</v>
       </c>
       <c r="H207">
-        <v>0.25024326553560899</v>
+        <v>0.25652097655190098</v>
       </c>
       <c r="I207">
         <v>-0.20507360226177199</v>
@@ -8398,7 +8398,7 @@
         <v>0.326901535211505</v>
       </c>
       <c r="H208">
-        <v>0.31795994448697201</v>
+        <v>0.32663207650790599</v>
       </c>
       <c r="I208">
         <v>-0.267561972751789</v>
@@ -8433,7 +8433,7 @@
         <v>0.28132710806575301</v>
       </c>
       <c r="H209">
-        <v>0.210713452126079</v>
+        <v>0.22242015570022</v>
       </c>
       <c r="I209">
         <v>-0.19831446956632001</v>
@@ -8468,7 +8468,7 @@
         <v>0.25583418603900698</v>
       </c>
       <c r="H210">
-        <v>0.180349699891799</v>
+        <v>0.18774796300033</v>
       </c>
       <c r="I210">
         <v>-0.21874331742598899</v>
@@ -8503,7 +8503,7 @@
         <v>0.352932438622164</v>
       </c>
       <c r="H211">
-        <v>0.301832704743072</v>
+        <v>0.30315756694968499</v>
       </c>
       <c r="I211">
         <v>-0.26426877650778602</v>
@@ -8538,7 +8538,7 @@
         <v>0.25871717477656198</v>
       </c>
       <c r="H212">
-        <v>0.22978715014787099</v>
+        <v>0.23930818585212299</v>
       </c>
       <c r="I212">
         <v>-0.19655767719866499</v>
@@ -8573,7 +8573,7 @@
         <v>0.116672852001573</v>
       </c>
       <c r="H213">
-        <v>9.28291073282317E-2</v>
+        <v>0.11262777880713799</v>
       </c>
       <c r="I213">
         <v>-8.76443367694026E-2</v>
@@ -8608,7 +8608,7 @@
         <v>0.27892575097079397</v>
       </c>
       <c r="H214">
-        <v>0.26695020551718701</v>
+        <v>0.28018772258476499</v>
       </c>
       <c r="I214">
         <v>-0.17707705881911001</v>
@@ -8643,7 +8643,7 @@
         <v>0.20516096162993899</v>
       </c>
       <c r="H215">
-        <v>0.19895881810891999</v>
+        <v>0.20169378516070699</v>
       </c>
       <c r="I215">
         <v>-0.159519428416697</v>
@@ -8678,7 +8678,7 @@
         <v>3.9962844252088301E-3</v>
       </c>
       <c r="H216">
-        <v>4.4088765490067898E-2</v>
+        <v>9.9942156802700105E-2</v>
       </c>
       <c r="I216">
         <v>-4.8191209195027E-2</v>
@@ -8713,7 +8713,7 @@
         <v>0.27113060750842</v>
       </c>
       <c r="H217">
-        <v>0.22089121268454401</v>
+        <v>0.23305498464260099</v>
       </c>
       <c r="I217">
         <v>-0.23032514666661699</v>
@@ -8748,7 +8748,7 @@
         <v>0.32209717005332</v>
       </c>
       <c r="H218">
-        <v>0.33289396771472102</v>
+        <v>0.33996794635203298</v>
       </c>
       <c r="I218">
         <v>-0.30056466148593097</v>
@@ -8783,7 +8783,7 @@
         <v>0.23623890431120201</v>
       </c>
       <c r="H219">
-        <v>0.213061405645256</v>
+        <v>0.217182162682267</v>
       </c>
       <c r="I219">
         <v>-0.139388673193825</v>
@@ -8818,7 +8818,7 @@
         <v>5.0125859231293602E-3</v>
       </c>
       <c r="H220">
-        <v>-3.3939117325699097E-2</v>
+        <v>-4.2589864874210001E-2</v>
       </c>
       <c r="I220">
         <v>-4.3197723469289101E-2</v>
@@ -8853,7 +8853,7 @@
         <v>0.29162600952832901</v>
       </c>
       <c r="H221">
-        <v>0.29014260316087498</v>
+        <v>0.29941983850978798</v>
       </c>
       <c r="I221">
         <v>-0.18839527576351101</v>
@@ -8888,7 +8888,7 @@
         <v>0.25777303462988099</v>
       </c>
       <c r="H222">
-        <v>0.23846305120319</v>
+        <v>0.24323082674705901</v>
       </c>
       <c r="I222">
         <v>-0.15222848553788301</v>
@@ -8923,7 +8923,7 @@
         <v>0.351857645077715</v>
       </c>
       <c r="H223">
-        <v>0.31797267626356901</v>
+        <v>0.32520884008890899</v>
       </c>
       <c r="I223">
         <v>-0.27424569869361898</v>
@@ -8958,7 +8958,7 @@
         <v>0.200294593369334</v>
       </c>
       <c r="H224">
-        <v>0.188437142288848</v>
+        <v>0.19679476365298401</v>
       </c>
       <c r="I224">
         <v>-0.11101499568689099</v>
@@ -8993,7 +8993,7 @@
         <v>0.241748224018663</v>
       </c>
       <c r="H225">
-        <v>0.243959330553492</v>
+        <v>0.24828185116930601</v>
       </c>
       <c r="I225">
         <v>-0.20852514933876201</v>
@@ -9028,7 +9028,7 @@
         <v>0.333278170534761</v>
       </c>
       <c r="H226">
-        <v>0.30371995660623302</v>
+        <v>0.30057064872733003</v>
       </c>
       <c r="I226">
         <v>-0.31828412963160502</v>
@@ -9063,7 +9063,7 @@
         <v>0.30004534185853898</v>
       </c>
       <c r="H227">
-        <v>0.23764270124214101</v>
+        <v>0.26550564516851</v>
       </c>
       <c r="I227">
         <v>-0.23136141212563299</v>
@@ -9098,7 +9098,7 @@
         <v>0.248176794299445</v>
       </c>
       <c r="H228">
-        <v>0.225488600947962</v>
+        <v>0.242814841321639</v>
       </c>
       <c r="I228">
         <v>-0.16688612869133401</v>
@@ -9133,7 +9133,7 @@
         <v>0.14671426742415999</v>
       </c>
       <c r="H229">
-        <v>0.11998419568173101</v>
+        <v>5.27685023115083E-2</v>
       </c>
       <c r="I229">
         <v>-0.15417839846565201</v>
@@ -9168,7 +9168,7 @@
         <v>0.22370935940580799</v>
       </c>
       <c r="H230">
-        <v>0.23643059578603301</v>
+        <v>0.24638966225146899</v>
       </c>
       <c r="I230">
         <v>-8.2933247091688103E-2</v>
@@ -9203,7 +9203,7 @@
         <v>0.19741376472873101</v>
       </c>
       <c r="H231">
-        <v>0.179325959440677</v>
+        <v>0.166708079498433</v>
       </c>
       <c r="I231">
         <v>-0.110145797007696</v>
@@ -9238,7 +9238,7 @@
         <v>0.32174049942823801</v>
       </c>
       <c r="H232">
-        <v>0.30069367803100799</v>
+        <v>0.29071930763503001</v>
       </c>
       <c r="I232">
         <v>-0.271655715634392</v>
@@ -9273,7 +9273,7 @@
         <v>0.26453297542881898</v>
       </c>
       <c r="H233">
-        <v>0.25533378869606199</v>
+        <v>0.26469924844682802</v>
       </c>
       <c r="I233">
         <v>-0.226434094227081</v>
@@ -9308,7 +9308,7 @@
         <v>0.318704567948496</v>
       </c>
       <c r="H234">
-        <v>0.31304944031251097</v>
+        <v>0.31365848045302502</v>
       </c>
       <c r="I234">
         <v>-0.32816549276518497</v>
@@ -9343,7 +9343,7 @@
         <v>0.232366471751599</v>
       </c>
       <c r="H235">
-        <v>0.23001612103494101</v>
+        <v>0.22974680153942001</v>
       </c>
       <c r="I235">
         <v>-0.20887163306216799</v>
@@ -9378,7 +9378,7 @@
         <v>0.40160776398471498</v>
       </c>
       <c r="H236">
-        <v>0.365617631668052</v>
+        <v>0.36162846677132399</v>
       </c>
       <c r="I236">
         <v>-0.33841485605231097</v>
@@ -9413,7 +9413,7 @@
         <v>0.44056711321904601</v>
       </c>
       <c r="H237">
-        <v>0.38362973718555099</v>
+        <v>0.36079959993798399</v>
       </c>
       <c r="I237">
         <v>-0.36341241238114802</v>
@@ -9448,7 +9448,7 @@
         <v>2.5104845064809499E-2</v>
       </c>
       <c r="H238">
-        <v>-6.4445503211021396E-2</v>
+        <v>2.1398356898941099E-2</v>
       </c>
       <c r="I238">
         <v>-2.47064428764232E-2</v>
@@ -9483,7 +9483,7 @@
         <v>0.25183636517289198</v>
       </c>
       <c r="H239">
-        <v>0.25652097655190098</v>
+        <v>0.25696376398398602</v>
       </c>
       <c r="I239">
         <v>-0.18828828468455699</v>
@@ -9518,7 +9518,7 @@
         <v>0.325152369280644</v>
       </c>
       <c r="H240">
-        <v>0.32663207650790599</v>
+        <v>0.30301344999082103</v>
       </c>
       <c r="I240">
         <v>-0.28931007040866802</v>
@@ -9553,7 +9553,7 @@
         <v>0.286750549971167</v>
       </c>
       <c r="H241">
-        <v>0.22242015570022</v>
+        <v>0.23688393316558601</v>
       </c>
       <c r="I241">
         <v>-0.20405882031419501</v>
@@ -9588,7 +9588,7 @@
         <v>0.25979288724701599</v>
       </c>
       <c r="H242">
-        <v>0.18774796300033</v>
+        <v>0.15361174658118101</v>
       </c>
       <c r="I242">
         <v>-0.209507729461965</v>
@@ -9623,7 +9623,7 @@
         <v>0.33083942371275499</v>
       </c>
       <c r="H243">
-        <v>0.30315756694968499</v>
+        <v>0.315202543715697</v>
       </c>
       <c r="I243">
         <v>-0.27034560389078399</v>
@@ -9658,7 +9658,7 @@
         <v>0.26480516387182401</v>
       </c>
       <c r="H244">
-        <v>0.23930818585212299</v>
+        <v>0.20941750056606201</v>
       </c>
       <c r="I244">
         <v>-0.18924724902085399</v>
@@ -9693,7 +9693,7 @@
         <v>0.118427884030643</v>
       </c>
       <c r="H245">
-        <v>0.11262777880713799</v>
+        <v>0.11477342492303701</v>
       </c>
       <c r="I245">
         <v>-8.5052010228948496E-2</v>
@@ -9728,7 +9728,7 @@
         <v>0.29071729494731702</v>
       </c>
       <c r="H246">
-        <v>0.28018772258476499</v>
+        <v>0.28203808964869598</v>
       </c>
       <c r="I246">
         <v>-0.24844849097977001</v>
@@ -9763,7 +9763,7 @@
         <v>0.20614541174551701</v>
       </c>
       <c r="H247">
-        <v>0.20169378516070699</v>
+        <v>0.192016933050773</v>
       </c>
       <c r="I247">
         <v>-0.17554049988447301</v>
@@ -9798,7 +9798,7 @@
         <v>6.5791192862830097E-2</v>
       </c>
       <c r="H248">
-        <v>9.9942156802700105E-2</v>
+        <v>1.12144349400132E-2</v>
       </c>
       <c r="I248">
         <v>-6.6140293571239003E-2</v>
@@ -9833,7 +9833,7 @@
         <v>0.274243855509061</v>
       </c>
       <c r="H249">
-        <v>0.23305498464260099</v>
+        <v>0.23902824729845501</v>
       </c>
       <c r="I249">
         <v>-0.240224825861553</v>
@@ -9868,7 +9868,7 @@
         <v>0.32455338989210603</v>
       </c>
       <c r="H250">
-        <v>0.33996794635203298</v>
+        <v>0.33177523077580101</v>
       </c>
       <c r="I250">
         <v>-0.30683427979764499</v>
@@ -9903,7 +9903,7 @@
         <v>0.23466729859455299</v>
       </c>
       <c r="H251">
-        <v>0.217182162682267</v>
+        <v>0.22137279192530299</v>
       </c>
       <c r="I251">
         <v>-0.160862707524034</v>
@@ -9938,7 +9938,7 @@
         <v>-6.0939034341590301E-2</v>
       </c>
       <c r="H252">
-        <v>-4.2589864874210001E-2</v>
+        <v>8.6313845898509101E-3</v>
       </c>
       <c r="I252">
         <v>-4.5565882466840797E-2</v>
@@ -9973,7 +9973,7 @@
         <v>0.25953400598516502</v>
       </c>
       <c r="H253">
-        <v>0.29941983850978798</v>
+        <v>0.29739148634088902</v>
       </c>
       <c r="I253">
         <v>-0.208177654962616</v>
@@ -10008,7 +10008,7 @@
         <v>0.25441542271707701</v>
       </c>
       <c r="H254">
-        <v>0.24323082674705901</v>
+        <v>0.21606766909705</v>
       </c>
       <c r="I254">
         <v>-0.135600923492493</v>
@@ -10043,7 +10043,7 @@
         <v>0.34311193211339103</v>
       </c>
       <c r="H255">
-        <v>0.32520884008890899</v>
+        <v>0.31827307456180298</v>
       </c>
       <c r="I255">
         <v>-0.30480725376921303</v>
@@ -10078,7 +10078,7 @@
         <v>0.20188939559233501</v>
       </c>
       <c r="H256">
-        <v>0.19679476365298401</v>
+        <v>0.17992072969544001</v>
       </c>
       <c r="I256">
         <v>-0.17357863807274801</v>
@@ -10113,7 +10113,7 @@
         <v>0.24848213195924601</v>
       </c>
       <c r="H257">
-        <v>0.24828185116930601</v>
+        <v>0.224226147135132</v>
       </c>
       <c r="I257">
         <v>-0.217899468783916</v>
@@ -10148,7 +10148,7 @@
         <v>0.34647421383214899</v>
       </c>
       <c r="H258">
-        <v>0.30057064872733003</v>
+        <v>0.28659608868237602</v>
       </c>
       <c r="I258">
         <v>-0.325819401633066</v>
@@ -10183,7 +10183,7 @@
         <v>0.28742088407222299</v>
       </c>
       <c r="H259">
-        <v>0.26550564516851</v>
+        <v>0.26356408787251301</v>
       </c>
       <c r="I259">
         <v>-0.242409520155492</v>
@@ -10218,7 +10218,7 @@
         <v>0.25960052275169199</v>
       </c>
       <c r="H260">
-        <v>0.242814841321639</v>
+        <v>0.25899099485806298</v>
       </c>
       <c r="I260">
         <v>-0.22609524789157201</v>
@@ -10253,7 +10253,7 @@
         <v>0.17452998315012599</v>
       </c>
       <c r="H261">
-        <v>5.27685023115083E-2</v>
+        <v>8.9089975002378793E-2</v>
       </c>
       <c r="I261">
         <v>-0.16714337127850501</v>
@@ -10288,7 +10288,7 @@
         <v>0.23050485734194501</v>
       </c>
       <c r="H262">
-        <v>0.24638966225146899</v>
+        <v>0.19095790720274</v>
       </c>
       <c r="I262">
         <v>-0.13122488133961999</v>
@@ -10323,7 +10323,7 @@
         <v>0.189693314211477</v>
       </c>
       <c r="H263">
-        <v>0.166708079498433</v>
+        <v>0.157554278122674</v>
       </c>
       <c r="I263">
         <v>-0.133628711106105</v>
@@ -10358,7 +10358,7 @@
         <v>0.329290728133394</v>
       </c>
       <c r="H264">
-        <v>0.29071930763503001</v>
+        <v>0.31012748650373601</v>
       </c>
       <c r="I264">
         <v>-0.21852911669281699</v>
@@ -10393,7 +10393,7 @@
         <v>0.26960833957221703</v>
       </c>
       <c r="H265">
-        <v>0.26469924844682802</v>
+        <v>0.23342893545780199</v>
       </c>
       <c r="I265">
         <v>-0.20998916777031201</v>
@@ -10428,7 +10428,7 @@
         <v>0.33169617772959498</v>
       </c>
       <c r="H266">
-        <v>0.31365848045302502</v>
+        <v>0.31415731486187698</v>
       </c>
       <c r="I266">
         <v>-0.33940724140925999</v>
@@ -10463,7 +10463,7 @@
         <v>0.222352416938779</v>
       </c>
       <c r="H267">
-        <v>0.22974680153942001</v>
+        <v>0.22586418085698101</v>
       </c>
       <c r="I267">
         <v>-0.21780003434301001</v>
@@ -10498,7 +10498,7 @@
         <v>0.37228997972815497</v>
       </c>
       <c r="H268">
-        <v>0.36162846677132399</v>
+        <v>0.406979618220915</v>
       </c>
       <c r="I268">
         <v>-0.28434547445351699</v>
@@ -10533,7 +10533,7 @@
         <v>0.43621263915132902</v>
       </c>
       <c r="H269">
-        <v>0.36079959993798399</v>
+        <v>0.37436378452149199</v>
       </c>
       <c r="I269">
         <v>-0.37959160046411</v>
@@ -10568,7 +10568,7 @@
         <v>2.4630211682863399E-3</v>
       </c>
       <c r="H270">
-        <v>2.1398356898941099E-2</v>
+        <v>-1.9909964583657599E-3</v>
       </c>
       <c r="I270">
         <v>1.26419144754122E-2</v>
@@ -10603,7 +10603,7 @@
         <v>0.25598806817179398</v>
       </c>
       <c r="H271">
-        <v>0.25696376398398602</v>
+        <v>0.25189787197050101</v>
       </c>
       <c r="I271">
         <v>-0.20022140150220499</v>
@@ -10638,7 +10638,7 @@
         <v>0.311336232613591</v>
       </c>
       <c r="H272">
-        <v>0.30301344999082103</v>
+        <v>0.29924872004139802</v>
       </c>
       <c r="I272">
         <v>-0.265434880956956</v>
@@ -10673,7 +10673,7 @@
         <v>0.27064620426081398</v>
       </c>
       <c r="H273">
-        <v>0.23688393316558601</v>
+        <v>0.20962043601889499</v>
       </c>
       <c r="I273">
         <v>-0.229558086019793</v>
@@ -10708,7 +10708,7 @@
         <v>0.25542446107977002</v>
       </c>
       <c r="H274">
-        <v>0.15361174658118101</v>
+        <v>0.165921446568078</v>
       </c>
       <c r="I274">
         <v>-0.206301473316472</v>
@@ -10743,7 +10743,7 @@
         <v>0.35232380817581499</v>
       </c>
       <c r="H275">
-        <v>0.315202543715697</v>
+        <v>0.26999420047535699</v>
       </c>
       <c r="I275">
         <v>-0.26891168235787</v>
@@ -10778,7 +10778,7 @@
         <v>0.26229517859878199</v>
       </c>
       <c r="H276">
-        <v>0.20941750056606201</v>
+        <v>0.18915764153745299</v>
       </c>
       <c r="I276">
         <v>-0.224955430168049</v>
@@ -10813,7 +10813,7 @@
         <v>0.135177665714448</v>
       </c>
       <c r="H277">
-        <v>0.11477342492303701</v>
+        <v>0.106969396010399</v>
       </c>
       <c r="I277">
         <v>-6.2722100728432706E-2</v>
@@ -10848,7 +10848,7 @@
         <v>0.288862861448484</v>
       </c>
       <c r="H278">
-        <v>0.28203808964869598</v>
+        <v>0.27192208236752102</v>
       </c>
       <c r="I278">
         <v>-0.25874324083331901</v>
@@ -10883,7 +10883,7 @@
         <v>0.209543460257752</v>
       </c>
       <c r="H279">
-        <v>0.192016933050773</v>
+        <v>0.18773796844958601</v>
       </c>
       <c r="I279">
         <v>-0.17850890711039499</v>
@@ -10918,7 +10918,7 @@
         <v>6.5791192862830097E-2</v>
       </c>
       <c r="H280">
-        <v>1.12144349400132E-2</v>
+        <v>6.5791192862830097E-2</v>
       </c>
       <c r="I280">
         <v>-9.7249045587244606E-2</v>
@@ -10953,7 +10953,7 @@
         <v>0.27127363233145002</v>
       </c>
       <c r="H281">
-        <v>0.23902824729845501</v>
+        <v>0.247376227614861</v>
       </c>
       <c r="I281">
         <v>-0.21542019348709801</v>
@@ -10988,7 +10988,7 @@
         <v>0.33429812310738999</v>
       </c>
       <c r="H282">
-        <v>0.33177523077580101</v>
+        <v>0.339734363541284</v>
       </c>
       <c r="I282">
         <v>-0.29404569020058002</v>
@@ -11023,7 +11023,7 @@
         <v>0.23381471043228599</v>
       </c>
       <c r="H283">
-        <v>0.22137279192530299</v>
+        <v>0.195690023848757</v>
       </c>
       <c r="I283">
         <v>-0.17329540967681101</v>
@@ -11058,7 +11058,7 @@
         <v>-1.1002309724355E-3</v>
       </c>
       <c r="H284">
-        <v>8.6313845898509101E-3</v>
+        <v>9.6833810491957301E-2</v>
       </c>
       <c r="I284">
         <v>-7.1576905522592299E-2</v>
@@ -11093,7 +11093,7 @@
         <v>0.25637070758293701</v>
       </c>
       <c r="H285">
-        <v>0.29739148634088902</v>
+        <v>0.27839264012841097</v>
       </c>
       <c r="I285">
         <v>-0.235571535255302</v>
@@ -11128,7 +11128,7 @@
         <v>0.24845378893858</v>
       </c>
       <c r="H286">
-        <v>0.21606766909705</v>
+        <v>0.22909754197631901</v>
       </c>
       <c r="I286">
         <v>-0.114790957028163</v>
@@ -11163,7 +11163,7 @@
         <v>0.35269205890713301</v>
       </c>
       <c r="H287">
-        <v>0.31827307456180298</v>
+        <v>0.33089219124605901</v>
       </c>
       <c r="I287">
         <v>-0.32788545605671898</v>
@@ -11198,7 +11198,7 @@
         <v>0.21059271984564301</v>
       </c>
       <c r="H288">
-        <v>0.17992072969544001</v>
+        <v>0.164839224517532</v>
       </c>
       <c r="I288">
         <v>-0.170094270345445</v>
@@ -11233,7 +11233,7 @@
         <v>0.24924926570725101</v>
       </c>
       <c r="H289">
-        <v>0.224226147135132</v>
+        <v>0.19759837719047699</v>
       </c>
       <c r="I289">
         <v>-0.21296082769899399</v>
@@ -11268,7 +11268,7 @@
         <v>0.34070398756925602</v>
       </c>
       <c r="H290">
-        <v>0.30166744685475799</v>
+        <v>0.34292343340583298</v>
       </c>
       <c r="I290">
         <v>-0.331392493749536</v>
@@ -11303,7 +11303,7 @@
         <v>0.27575619130267598</v>
       </c>
       <c r="H291">
-        <v>0.24815983629069299</v>
+        <v>0.26694211182858402</v>
       </c>
       <c r="I291">
         <v>-0.16920575449511299</v>
@@ -11338,7 +11338,7 @@
         <v>0.25763816987600502</v>
       </c>
       <c r="H292">
-        <v>0.27168714638076702</v>
+        <v>0.270198232558087</v>
       </c>
       <c r="I292">
         <v>-0.176669720275758</v>
@@ -11373,7 +11373,7 @@
         <v>0.199439251701298</v>
       </c>
       <c r="H293">
-        <v>8.9093108426892401E-2</v>
+        <v>0.15032224054658999</v>
       </c>
       <c r="I293">
         <v>-0.18460965623688</v>
@@ -11408,7 +11408,7 @@
         <v>0.25475321704832299</v>
       </c>
       <c r="H294">
-        <v>0.19628853920744799</v>
+        <v>0.21271085602491099</v>
       </c>
       <c r="I294">
         <v>-0.14000036126358201</v>
@@ -11443,7 +11443,7 @@
         <v>0.202628655235742</v>
       </c>
       <c r="H295">
-        <v>0.15705888041003199</v>
+        <v>0.16787808795331699</v>
       </c>
       <c r="I295">
         <v>-0.117031367640362</v>
@@ -11478,7 +11478,7 @@
         <v>0.33688401452233502</v>
       </c>
       <c r="H296">
-        <v>0.311295868059414</v>
+        <v>0.25310225708858303</v>
       </c>
       <c r="I296">
         <v>-0.22796340319137101</v>
@@ -11513,7 +11513,7 @@
         <v>0.28646833912354303</v>
       </c>
       <c r="H297">
-        <v>0.24516071236779</v>
+        <v>0.22385401178599601</v>
       </c>
       <c r="I297">
         <v>-0.195731654404177</v>
@@ -11548,7 +11548,7 @@
         <v>0.35148907387892703</v>
       </c>
       <c r="H298">
-        <v>0.33421303498240601</v>
+        <v>0.29997360973604797</v>
       </c>
       <c r="I298">
         <v>-0.336494211793602</v>
@@ -11583,7 +11583,7 @@
         <v>0.21471487393066499</v>
       </c>
       <c r="H299">
-        <v>0.21319803187873301</v>
+        <v>0.19109664466558501</v>
       </c>
       <c r="I299">
         <v>-0.20160250546540001</v>
@@ -11618,7 +11618,7 @@
         <v>0.37143575987066701</v>
       </c>
       <c r="H300">
-        <v>0.41185737730307698</v>
+        <v>0.34340749935489201</v>
       </c>
       <c r="I300">
         <v>-0.27063541583725498</v>
@@ -11653,7 +11653,7 @@
         <v>0.42239302016990599</v>
       </c>
       <c r="H301">
-        <v>0.36901840365926097</v>
+        <v>0.36853031919281398</v>
       </c>
       <c r="I301">
         <v>-0.36337416369554598</v>
@@ -11688,7 +11688,7 @@
         <v>-6.1863638106996799E-2</v>
       </c>
       <c r="H302">
-        <v>3.1573331002462603E-2</v>
+        <v>4.8225892189338398E-2</v>
       </c>
       <c r="I302">
         <v>2.2928021843053401E-2</v>
@@ -11723,7 +11723,7 @@
         <v>0.24109571188571599</v>
       </c>
       <c r="H303">
-        <v>0.24274787262819</v>
+        <v>0.25887526927146698</v>
       </c>
       <c r="I303">
         <v>-0.22557427059249399</v>
@@ -11758,7 +11758,7 @@
         <v>0.31745475723104</v>
       </c>
       <c r="H304">
-        <v>0.30139855882954703</v>
+        <v>0.30939564416035398</v>
       </c>
       <c r="I304">
         <v>-0.27536544288026499</v>
@@ -11793,7 +11793,7 @@
         <v>0.27788849576249702</v>
       </c>
       <c r="H305">
-        <v>0.215212754951665</v>
+        <v>0.226129931072407</v>
       </c>
       <c r="I305">
         <v>-0.21925106878839501</v>
@@ -11828,7 +11828,7 @@
         <v>0.25183424371625002</v>
       </c>
       <c r="H306">
-        <v>0.19253506566617801</v>
+        <v>0.19383356772025501</v>
       </c>
       <c r="I306">
         <v>-0.15861296311241799</v>
@@ -11863,7 +11863,7 @@
         <v>0.36777404050422702</v>
       </c>
       <c r="H307">
-        <v>0.28450252445060598</v>
+        <v>0.26933196606376802</v>
       </c>
       <c r="I307">
         <v>-0.30394972900087702</v>
@@ -11898,7 +11898,7 @@
         <v>0.27805755637004897</v>
       </c>
       <c r="H308">
-        <v>0.19442004183527201</v>
+        <v>0.13159502244402899</v>
       </c>
       <c r="I308">
         <v>-0.25233026280451698</v>
@@ -11933,7 +11933,7 @@
         <v>0.11481202490631</v>
       </c>
       <c r="H309">
-        <v>9.7188012965377296E-2</v>
+        <v>0.14839088659958899</v>
       </c>
       <c r="I309">
         <v>-6.3772392470013997E-2</v>
@@ -11968,7 +11968,7 @@
         <v>0.29506974319936702</v>
       </c>
       <c r="H310">
-        <v>0.27591796439826899</v>
+        <v>0.26250064672463902</v>
       </c>
       <c r="I310">
         <v>-0.21028032774211899</v>
@@ -12003,7 +12003,7 @@
         <v>0.217071216205319</v>
       </c>
       <c r="H311">
-        <v>0.202822296721692</v>
+        <v>0.18876599070627301</v>
       </c>
       <c r="I311">
         <v>-0.17717008699006701</v>
@@ -12073,7 +12073,7 @@
         <v>0.26395544549609801</v>
       </c>
       <c r="H313">
-        <v>0.23942373759669</v>
+        <v>0.20554962467492299</v>
       </c>
       <c r="I313">
         <v>-0.187917429063335</v>
@@ -12108,7 +12108,7 @@
         <v>0.35181059717450602</v>
       </c>
       <c r="H314">
-        <v>0.34594270494100798</v>
+        <v>0.31413027985140501</v>
       </c>
       <c r="I314">
         <v>-0.31406346357797199</v>
@@ -12143,7 +12143,7 @@
         <v>0.23253035449697301</v>
       </c>
       <c r="H315">
-        <v>0.21284252996980901</v>
+        <v>0.224206616812577</v>
       </c>
       <c r="I315">
         <v>-0.20861010391731399</v>
@@ -12178,7 +12178,7 @@
         <v>7.6637383937893294E-2</v>
       </c>
       <c r="H316">
-        <v>9.4800512457558397E-2</v>
+        <v>4.9869238324246702E-2</v>
       </c>
       <c r="I316">
         <v>-8.44835479810013E-2</v>
@@ -12213,7 +12213,7 @@
         <v>0.28322686668598401</v>
       </c>
       <c r="H317">
-        <v>0.29639921336311997</v>
+        <v>0.32729892129833099</v>
       </c>
       <c r="I317">
         <v>-0.27456056242225801</v>
@@ -12248,7 +12248,7 @@
         <v>0.25784650106064799</v>
       </c>
       <c r="H318">
-        <v>0.24257035689727499</v>
+        <v>0.22933479438773199</v>
       </c>
       <c r="I318">
         <v>-0.13734116247897199</v>
@@ -12283,7 +12283,7 @@
         <v>0.35459963483176299</v>
       </c>
       <c r="H319">
-        <v>0.33271719041987202</v>
+        <v>0.33185525045467301</v>
       </c>
       <c r="I319">
         <v>-0.31058830389715297</v>
@@ -12318,7 +12318,7 @@
         <v>0.20780185044872199</v>
       </c>
       <c r="H320">
-        <v>0.18114943306258599</v>
+        <v>0.20638462223160101</v>
       </c>
       <c r="I320">
         <v>-0.14954304471183499</v>
@@ -12353,7 +12353,7 @@
         <v>0.26125822518471697</v>
       </c>
       <c r="H321">
-        <v>0.21721896947262201</v>
+        <v>0.27016766122117097</v>
       </c>
       <c r="I321">
         <v>-0.23609793617757399</v>
@@ -12388,7 +12388,7 @@
         <v>0.34337032066010997</v>
       </c>
       <c r="H322">
-        <v>-7.3980267591480199E-3</v>
+        <v>0.33189683873050402</v>
       </c>
       <c r="I322">
         <v>-0.29178983802388497</v>
@@ -12423,7 +12423,7 @@
         <v>0.27120895644061699</v>
       </c>
       <c r="H323">
-        <v>5.8058084081345399E-2</v>
+        <v>0.20305654145205701</v>
       </c>
       <c r="I323">
         <v>-0.22363660926573201</v>
@@ -12458,7 +12458,7 @@
         <v>0.27230271694728198</v>
       </c>
       <c r="H324">
-        <v>-8.49926001008416E-2</v>
+        <v>0.248270093230467</v>
       </c>
       <c r="I324">
         <v>-0.21364034675928201</v>
@@ -12493,7 +12493,7 @@
         <v>0.195098793008146</v>
       </c>
       <c r="H325">
-        <v>-5.5224234378728802E-2</v>
+        <v>8.8555664796977004E-2</v>
       </c>
       <c r="I325">
         <v>-0.159354979747547</v>
@@ -12528,7 +12528,7 @@
         <v>0.265343356614679</v>
       </c>
       <c r="H326">
-        <v>0.14843672487739301</v>
+        <v>0.20681355209781299</v>
       </c>
       <c r="I326">
         <v>-0.16306203911275199</v>
@@ -12563,7 +12563,7 @@
         <v>0.20211308144671999</v>
       </c>
       <c r="H327">
-        <v>5.3387080005093103E-2</v>
+        <v>0.162797178942645</v>
       </c>
       <c r="I327">
         <v>-0.14117012726213801</v>
@@ -12598,7 +12598,7 @@
         <v>0.35128190121819503</v>
       </c>
       <c r="H328">
-        <v>3.8199876775996303E-2</v>
+        <v>0.30980207895957801</v>
       </c>
       <c r="I328">
         <v>-0.252720078715793</v>
@@ -12633,7 +12633,7 @@
         <v>0.29073333555226599</v>
       </c>
       <c r="H329">
-        <v>-4.7923617737341197E-2</v>
+        <v>0.23565843410342099</v>
       </c>
       <c r="I329">
         <v>-0.23180056744081101</v>
@@ -12668,7 +12668,7 @@
         <v>0.31679998846186502</v>
       </c>
       <c r="H330">
-        <v>-0.160442544129101</v>
+        <v>0.30794222420662698</v>
       </c>
       <c r="I330">
         <v>-0.36257337621115399</v>
@@ -12703,7 +12703,7 @@
         <v>0.20561280993080899</v>
       </c>
       <c r="H331">
-        <v>6.0769265788445999E-2</v>
+        <v>0.18954200911442101</v>
       </c>
       <c r="I331">
         <v>-0.19158745827885701</v>
@@ -12738,7 +12738,7 @@
         <v>0.372173352444296</v>
       </c>
       <c r="H332">
-        <v>-4.8885187441172196E-4</v>
+        <v>0.38725499729268598</v>
       </c>
       <c r="I332">
         <v>-0.30186214061706601</v>
@@ -12773,7 +12773,7 @@
         <v>0.42655516206155403</v>
       </c>
       <c r="H333">
-        <v>6.9452848023701099E-3</v>
+        <v>0.36173032245977099</v>
       </c>
       <c r="I333">
         <v>-0.35740229590481898</v>
@@ -12808,7 +12808,7 @@
         <v>-6.7587373063354897E-2</v>
       </c>
       <c r="H334">
-        <v>3.5772891153564398E-2</v>
+        <v>7.21623150711714E-3</v>
       </c>
       <c r="I334">
         <v>5.6347831664034197E-3</v>
@@ -12843,7 +12843,7 @@
         <v>0.23769906386967499</v>
       </c>
       <c r="H335">
-        <v>4.0285969244063601E-2</v>
+        <v>0.22320478506615499</v>
       </c>
       <c r="I335">
         <v>-0.173211895621455</v>
@@ -12878,7 +12878,7 @@
         <v>0.32103658668704999</v>
       </c>
       <c r="H336">
-        <v>0.106626417112153</v>
+        <v>0.28997269651652102</v>
       </c>
       <c r="I336">
         <v>-0.2811566816785</v>
@@ -12913,7 +12913,7 @@
         <v>0.27346629184217602</v>
       </c>
       <c r="H337">
-        <v>8.4851698654375696E-2</v>
+        <v>0.255253627231461</v>
       </c>
       <c r="I337">
         <v>-0.238207288968347</v>
@@ -12948,7 +12948,7 @@
         <v>0.24233658474459899</v>
       </c>
       <c r="H338">
-        <v>-6.1470480666628198E-2</v>
+        <v>0.17747057696447399</v>
       </c>
       <c r="I338">
         <v>-0.19888248734403599</v>
@@ -12983,7 +12983,7 @@
         <v>0.37580341788072202</v>
       </c>
       <c r="H339">
-        <v>0.198843420279363</v>
+        <v>0.31449515233623998</v>
       </c>
       <c r="I339">
         <v>-0.288972989206918</v>
@@ -13018,7 +13018,7 @@
         <v>0.28155798931998299</v>
       </c>
       <c r="H340">
-        <v>-0.108023929293817</v>
+        <v>0.20139427736940799</v>
       </c>
       <c r="I340">
         <v>-0.25049336338950601</v>
@@ -13053,7 +13053,7 @@
         <v>0.113237080979296</v>
       </c>
       <c r="H341">
-        <v>8.6213054095713601E-2</v>
+        <v>0.14627030254603601</v>
       </c>
       <c r="I341">
         <v>-9.9724328317230396E-2</v>
@@ -13088,7 +13088,7 @@
         <v>0.30317836826745498</v>
       </c>
       <c r="H342">
-        <v>-7.7124176388281302E-3</v>
+        <v>0.236147835298711</v>
       </c>
       <c r="I342">
         <v>-0.252080839158216</v>
@@ -13123,7 +13123,7 @@
         <v>0.210425206484981</v>
       </c>
       <c r="H343">
-        <v>1.3526144175561E-2</v>
+        <v>0.18314905152101699</v>
       </c>
       <c r="I343">
         <v>-0.192089123485403</v>
@@ -13158,7 +13158,7 @@
         <v>3.1486878083113498E-2</v>
       </c>
       <c r="H344">
-        <v>0.15227108403092701</v>
+        <v>0.102861144675868</v>
       </c>
       <c r="I344">
         <v>-0.119087260928962</v>
@@ -13193,7 +13193,7 @@
         <v>0.27348738220136898</v>
       </c>
       <c r="H345">
-        <v>9.4285153921918094E-2</v>
+        <v>0.26479679509215998</v>
       </c>
       <c r="I345">
         <v>-0.22581847265138</v>
@@ -13228,7 +13228,7 @@
         <v>0.34635220951338902</v>
       </c>
       <c r="H346">
-        <v>0.100081011907172</v>
+        <v>0.29571933098741399</v>
       </c>
       <c r="I346">
         <v>-0.34117112226220803</v>
@@ -13263,7 +13263,7 @@
         <v>0.245612804545354</v>
       </c>
       <c r="H347">
-        <v>4.4013683646468797E-3</v>
+        <v>0.236845840827625</v>
       </c>
       <c r="I347">
         <v>-0.18827533128405299</v>
@@ -13298,7 +13298,7 @@
         <v>8.5646571215331604E-2</v>
       </c>
       <c r="H348">
-        <v>6.2753054264089905E-2</v>
+        <v>5.6487845961530302E-2</v>
       </c>
       <c r="I348">
         <v>-8.8879504838757797E-2</v>
@@ -13333,7 +13333,7 @@
         <v>0.29663656530135502</v>
       </c>
       <c r="H349">
-        <v>-1.3674920630434099E-2</v>
+        <v>0.311744202425421</v>
       </c>
       <c r="I349">
         <v>-0.28246258161959498</v>
@@ -13368,7 +13368,7 @@
         <v>0.251400850133425</v>
       </c>
       <c r="H350">
-        <v>4.5761747374303503E-2</v>
+        <v>0.204835537008837</v>
       </c>
       <c r="I350">
         <v>-0.19368912075829001</v>
@@ -13403,7 +13403,7 @@
         <v>0.34799295103815597</v>
       </c>
       <c r="H351">
-        <v>0.22177375147836101</v>
+        <v>0.324422177360283</v>
       </c>
       <c r="I351">
         <v>-0.27459719370710001</v>
@@ -13438,7 +13438,7 @@
         <v>0.211205892796859</v>
       </c>
       <c r="H352">
-        <v>7.9089192754176793E-2</v>
+        <v>0.162442600967208</v>
       </c>
       <c r="I352">
         <v>-0.135996134256646</v>
@@ -13473,7 +13473,7 @@
         <v>0.26520836635297201</v>
       </c>
       <c r="H353">
-        <v>8.6913570293157605E-2</v>
+        <v>0.23012670865547399</v>
       </c>
       <c r="I353">
         <v>-0.24932108484523999</v>
@@ -13502,13 +13502,13 @@
         <v>-0.30295304374399201</v>
       </c>
       <c r="F354">
-        <v>-0.37126255812133202</v>
+        <v>-0.363244877238177</v>
       </c>
       <c r="G354">
-        <v>0.34337032066010997</v>
+        <v>0.35912014260390301</v>
       </c>
       <c r="H354">
-        <v>0.33189683873050402</v>
+        <v>0.30992375486624402</v>
       </c>
       <c r="I354">
         <v>-0.33453327675903</v>
@@ -13537,13 +13537,13 @@
         <v>-0.255086617445066</v>
       </c>
       <c r="F355">
-        <v>-0.29925972432418002</v>
+        <v>-0.29955444122375902</v>
       </c>
       <c r="G355">
-        <v>0.27120895644061699</v>
+        <v>0.28249040717322799</v>
       </c>
       <c r="H355">
-        <v>0.20305654145205701</v>
+        <v>0.21505382645528601</v>
       </c>
       <c r="I355">
         <v>-0.159708632618209</v>
@@ -13572,13 +13572,13 @@
         <v>-0.28376936923180801</v>
       </c>
       <c r="F356">
-        <v>-0.30950482242639998</v>
+        <v>-0.295221227647949</v>
       </c>
       <c r="G356">
-        <v>0.27230271694728198</v>
+        <v>0.27797020214826601</v>
       </c>
       <c r="H356">
-        <v>0.248270093230467</v>
+        <v>0.264864983542688</v>
       </c>
       <c r="I356">
         <v>-0.25019441694231898</v>
@@ -13607,13 +13607,13 @@
         <v>-0.224757231832447</v>
       </c>
       <c r="F357">
-        <v>-0.13446084827725799</v>
+        <v>-9.2509318242914404E-2</v>
       </c>
       <c r="G357">
-        <v>0.195098793008146</v>
+        <v>0.185452620434893</v>
       </c>
       <c r="H357">
-        <v>8.8555664796977004E-2</v>
+        <v>0.100093821264926</v>
       </c>
       <c r="I357">
         <v>-0.12139776211144999</v>
@@ -13642,13 +13642,13 @@
         <v>-0.264419290886103</v>
       </c>
       <c r="F358">
-        <v>-0.27801245180987999</v>
+        <v>-0.26415360555396999</v>
       </c>
       <c r="G358">
-        <v>0.265343356614679</v>
+        <v>0.27685857902939298</v>
       </c>
       <c r="H358">
-        <v>0.20681355209781299</v>
+        <v>0.228909325864326</v>
       </c>
       <c r="I358">
         <v>-0.22572310510855401</v>
@@ -13677,13 +13677,13 @@
         <v>-0.174274439700255</v>
       </c>
       <c r="F359">
-        <v>-0.219360366827901</v>
+        <v>-0.184083803393538</v>
       </c>
       <c r="G359">
-        <v>0.20211308144671999</v>
+        <v>0.21435982928137601</v>
       </c>
       <c r="H359">
-        <v>0.162797178942645</v>
+        <v>0.18596083621951301</v>
       </c>
       <c r="I359">
         <v>-0.126042631051281</v>
@@ -13712,13 +13712,13 @@
         <v>-0.27701825799260699</v>
       </c>
       <c r="F360">
-        <v>-0.317768205323473</v>
+        <v>-0.32524018090110501</v>
       </c>
       <c r="G360">
-        <v>0.35128190121819503</v>
+        <v>0.35250381827727201</v>
       </c>
       <c r="H360">
-        <v>0.30980207895957801</v>
+        <v>0.28326514132664798</v>
       </c>
       <c r="I360">
         <v>-0.26709196900070398</v>
@@ -13747,13 +13747,13 @@
         <v>-0.25095689318139203</v>
       </c>
       <c r="F361">
-        <v>-0.28219456040659802</v>
+        <v>-0.28841451924082401</v>
       </c>
       <c r="G361">
-        <v>0.29073333555226599</v>
+        <v>0.27989431265986497</v>
       </c>
       <c r="H361">
-        <v>0.23565843410342099</v>
+        <v>0.24026804793939099</v>
       </c>
       <c r="I361">
         <v>-0.22098505164999999</v>
@@ -13782,13 +13782,13 @@
         <v>-0.254658692862611</v>
       </c>
       <c r="F362">
-        <v>-0.35442831584472101</v>
+        <v>-0.36471099338607998</v>
       </c>
       <c r="G362">
-        <v>0.31679998846186502</v>
+        <v>0.30940835284337398</v>
       </c>
       <c r="H362">
-        <v>0.30794222420662698</v>
+        <v>0.361291002672605</v>
       </c>
       <c r="I362">
         <v>-0.33538505450336098</v>
@@ -13817,13 +13817,13 @@
         <v>-0.23087823232004101</v>
       </c>
       <c r="F363">
-        <v>-0.21488559731531001</v>
+        <v>-0.220912708265362</v>
       </c>
       <c r="G363">
-        <v>0.20561280993080899</v>
+        <v>0.21666368504615699</v>
       </c>
       <c r="H363">
-        <v>0.18954200911442101</v>
+        <v>0.18985524961846101</v>
       </c>
       <c r="I363">
         <v>-0.17451722849006701</v>
@@ -13852,13 +13852,13 @@
         <v>-0.37608408637810697</v>
       </c>
       <c r="F364">
-        <v>-0.41520452595749502</v>
+        <v>-0.42629961971025099</v>
       </c>
       <c r="G364">
-        <v>0.372173352444296</v>
+        <v>0.36876337056372299</v>
       </c>
       <c r="H364">
-        <v>0.38725499729268598</v>
+        <v>0.35361934361397901</v>
       </c>
       <c r="I364">
         <v>-0.32288629034268101</v>
@@ -13887,13 +13887,13 @@
         <v>-0.37368362019340801</v>
       </c>
       <c r="F365">
-        <v>-0.447733667546654</v>
+        <v>-0.44362779776128702</v>
       </c>
       <c r="G365">
-        <v>0.42655516206155403</v>
+        <v>0.42681421208526199</v>
       </c>
       <c r="H365">
-        <v>0.36173032245977099</v>
+        <v>0.35409365521675101</v>
       </c>
       <c r="I365">
         <v>-0.35106660998316003</v>
@@ -13922,13 +13922,13 @@
         <v>-1.28357448502054E-2</v>
       </c>
       <c r="F366">
-        <v>-8.3436357848605702E-2</v>
+        <v>-0.12666836272446799</v>
       </c>
       <c r="G366">
-        <v>-6.7587373063354897E-2</v>
+        <v>-7.4013722657988402E-3</v>
       </c>
       <c r="H366">
-        <v>7.21623150711714E-3</v>
+        <v>1.34358691830649E-2</v>
       </c>
       <c r="I366">
         <v>3.2393705769475601E-3</v>
@@ -13957,13 +13957,13 @@
         <v>-0.18493786498821399</v>
       </c>
       <c r="F367">
-        <v>-0.273195091470605</v>
+        <v>-0.26253497248445401</v>
       </c>
       <c r="G367">
-        <v>0.23769906386967499</v>
+        <v>0.23537657142616</v>
       </c>
       <c r="H367">
-        <v>0.22320478506615499</v>
+        <v>0.225086414463185</v>
       </c>
       <c r="I367">
         <v>-0.192928855640181</v>
@@ -13992,13 +13992,13 @@
         <v>-0.31768321642017799</v>
       </c>
       <c r="F368">
-        <v>-0.36429992932970701</v>
+        <v>-0.360250685937689</v>
       </c>
       <c r="G368">
-        <v>0.32103658668704999</v>
+        <v>0.31084185247051699</v>
       </c>
       <c r="H368">
-        <v>0.28997269651652102</v>
+        <v>0.30278271789310202</v>
       </c>
       <c r="I368">
         <v>-0.27275344859289402</v>
@@ -14027,13 +14027,13 @@
         <v>-0.22842608561861499</v>
       </c>
       <c r="F369">
-        <v>-0.26029880418155199</v>
+        <v>-0.24869400738938199</v>
       </c>
       <c r="G369">
-        <v>0.27346629184217602</v>
+        <v>0.29444849354054298</v>
       </c>
       <c r="H369">
-        <v>0.255253627231461</v>
+        <v>0.20962491980534301</v>
       </c>
       <c r="I369">
         <v>-0.25799310139278497</v>
@@ -14062,13 +14062,13 @@
         <v>-0.22844232569141301</v>
       </c>
       <c r="F370">
-        <v>-0.23214390399518001</v>
+        <v>-0.20602717489400699</v>
       </c>
       <c r="G370">
-        <v>0.24233658474459899</v>
+        <v>0.252844112094046</v>
       </c>
       <c r="H370">
-        <v>0.17747057696447399</v>
+        <v>0.19779819010084099</v>
       </c>
       <c r="I370">
         <v>-0.16803608508260101</v>
@@ -14097,13 +14097,13 @@
         <v>-0.28455654255166102</v>
       </c>
       <c r="F371">
-        <v>-0.36830687069829199</v>
+        <v>-0.34810302328603998</v>
       </c>
       <c r="G371">
-        <v>0.37580341788072202</v>
+        <v>0.379587030488933</v>
       </c>
       <c r="H371">
-        <v>0.31449515233623998</v>
+        <v>0.249663650635741</v>
       </c>
       <c r="I371">
         <v>-0.35403414085825002</v>
@@ -14132,13 +14132,13 @@
         <v>-0.243824287706984</v>
       </c>
       <c r="F372">
-        <v>-0.29743949915703</v>
+        <v>-0.28291035621155902</v>
       </c>
       <c r="G372">
-        <v>0.28155798931998299</v>
+        <v>0.28249109288871699</v>
       </c>
       <c r="H372">
-        <v>0.20139427736940799</v>
+        <v>0.216916341198305</v>
       </c>
       <c r="I372">
         <v>-0.19039868783642</v>
@@ -14167,13 +14167,13 @@
         <v>-0.13074357376105999</v>
       </c>
       <c r="F373">
-        <v>-0.164961891908988</v>
+        <v>-0.173097165610094</v>
       </c>
       <c r="G373">
-        <v>0.113237080979296</v>
+        <v>0.114605321491316</v>
       </c>
       <c r="H373">
-        <v>0.14627030254603601</v>
+        <v>0.12284799293635899</v>
       </c>
       <c r="I373">
         <v>-6.9226325920186405E-2</v>
@@ -14202,13 +14202,13 @@
         <v>-0.26863596508586501</v>
       </c>
       <c r="F374">
-        <v>-0.30139383892994698</v>
+        <v>-0.29541091967112898</v>
       </c>
       <c r="G374">
-        <v>0.30317836826745498</v>
+        <v>0.30826536441119001</v>
       </c>
       <c r="H374">
-        <v>0.236147835298711</v>
+        <v>0.26571388283234898</v>
       </c>
       <c r="I374">
         <v>-0.21676733474170501</v>
@@ -14237,13 +14237,13 @@
         <v>-0.18582446969151101</v>
       </c>
       <c r="F375">
-        <v>-0.228907627418419</v>
+        <v>-0.22431720718596901</v>
       </c>
       <c r="G375">
-        <v>0.210425206484981</v>
+        <v>0.21057970350080901</v>
       </c>
       <c r="H375">
-        <v>0.18314905152101699</v>
+        <v>0.17938985047494799</v>
       </c>
       <c r="I375">
         <v>-0.18579672636589001</v>
@@ -14272,13 +14272,13 @@
         <v>-3.3557209398408901E-2</v>
       </c>
       <c r="F376">
-        <v>-1.24343151543838E-3</v>
+        <v>-3.3107523834437803E-2</v>
       </c>
       <c r="G376">
-        <v>3.1486878083113498E-2</v>
+        <v>-4.0350439421496E-2</v>
       </c>
       <c r="H376">
-        <v>0.102861144675868</v>
+        <v>0.100620567375887</v>
       </c>
       <c r="I376">
         <v>-3.3557209398408901E-2</v>
@@ -14307,13 +14307,13 @@
         <v>-0.24272764268868099</v>
       </c>
       <c r="F377">
-        <v>-0.283737323718741</v>
+        <v>-0.27979642897650903</v>
       </c>
       <c r="G377">
-        <v>0.27348738220136898</v>
+        <v>0.25781723239297499</v>
       </c>
       <c r="H377">
-        <v>0.26479679509215998</v>
+        <v>0.181012204688411</v>
       </c>
       <c r="I377">
         <v>-0.21179711009991201</v>
@@ -14342,13 +14342,13 @@
         <v>-0.26316386144836701</v>
       </c>
       <c r="F378">
-        <v>-0.36634556095582299</v>
+        <v>-0.351878315555814</v>
       </c>
       <c r="G378">
-        <v>0.34635220951338902</v>
+        <v>0.34204337718320199</v>
       </c>
       <c r="H378">
-        <v>0.29571933098741399</v>
+        <v>0.31973733331240201</v>
       </c>
       <c r="I378">
         <v>-0.30706136875135598</v>
@@ -14377,13 +14377,13 @@
         <v>-0.21809796012359201</v>
       </c>
       <c r="F379">
-        <v>-0.23917940716426001</v>
+        <v>-0.240250090861824</v>
       </c>
       <c r="G379">
-        <v>0.245612804545354</v>
+        <v>0.24211507885615199</v>
       </c>
       <c r="H379">
-        <v>0.236845840827625</v>
+        <v>0.200213872227641</v>
       </c>
       <c r="I379">
         <v>-0.16407357971466799</v>
@@ -14412,13 +14412,13 @@
         <v>-9.5802808875813994E-2</v>
       </c>
       <c r="F380">
-        <v>-0.102301192284214</v>
+        <v>-8.9747743397998098E-2</v>
       </c>
       <c r="G380">
-        <v>8.5646571215331604E-2</v>
+        <v>4.9754148226134602E-2</v>
       </c>
       <c r="H380">
-        <v>5.6487845961530302E-2</v>
+        <v>3.27839920369635E-2</v>
       </c>
       <c r="I380">
         <v>-6.8382414732160099E-2</v>
@@ -14447,13 +14447,13 @@
         <v>-0.26002498811487001</v>
       </c>
       <c r="F381">
-        <v>-0.33383374127676602</v>
+        <v>-0.313448515722691</v>
       </c>
       <c r="G381">
-        <v>0.29663656530135502</v>
+        <v>0.29730749235929099</v>
       </c>
       <c r="H381">
-        <v>0.311744202425421</v>
+        <v>0.277880377721761</v>
       </c>
       <c r="I381">
         <v>-0.244996757822143</v>
@@ -14482,13 +14482,13 @@
         <v>-0.212883970634515</v>
       </c>
       <c r="F382">
-        <v>-0.26819872912488302</v>
+        <v>-0.26224751643500699</v>
       </c>
       <c r="G382">
-        <v>0.251400850133425</v>
+        <v>0.252823852647378</v>
       </c>
       <c r="H382">
-        <v>0.204835537008837</v>
+        <v>0.20246532880072701</v>
       </c>
       <c r="I382">
         <v>-0.167248898926076</v>
@@ -14517,13 +14517,13 @@
         <v>-0.30527413272543402</v>
       </c>
       <c r="F383">
-        <v>-0.36425547484376702</v>
+        <v>-0.37005442936209798</v>
       </c>
       <c r="G383">
-        <v>0.34799295103815597</v>
+        <v>0.35799053992732299</v>
       </c>
       <c r="H383">
-        <v>0.324422177360283</v>
+        <v>0.32919268948908498</v>
       </c>
       <c r="I383">
         <v>-0.31046741391569699</v>
@@ -14552,13 +14552,13 @@
         <v>-0.16916716014233199</v>
       </c>
       <c r="F384">
-        <v>-0.23233304076366301</v>
+        <v>-0.227420721545668</v>
       </c>
       <c r="G384">
-        <v>0.211205892796859</v>
+        <v>0.20680585391822301</v>
       </c>
       <c r="H384">
-        <v>0.162442600967208</v>
+        <v>0.18386422850376799</v>
       </c>
       <c r="I384">
         <v>-0.120645510404358</v>
@@ -14587,13 +14587,13 @@
         <v>-0.25431509219825399</v>
       </c>
       <c r="F385">
-        <v>-0.28547293427922299</v>
+        <v>-0.27646412232504097</v>
       </c>
       <c r="G385">
-        <v>0.26520836635297201</v>
+        <v>0.261331118780046</v>
       </c>
       <c r="H385">
-        <v>0.23012670865547399</v>
+        <v>0.206553339452343</v>
       </c>
       <c r="I385">
         <v>-0.244940490744295</v>
@@ -14614,8 +14614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A352" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="A370" workbookViewId="0">
+      <selection activeCell="F354" sqref="F354:F385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27727,7 +27727,11 @@
       </c>
       <c r="F354">
         <f>'CPP Raw Data'!F354*-1</f>
-        <v>0.37126255812133202</v>
+        <v>0.363244877238177</v>
+      </c>
+      <c r="G354">
+        <f>'CPP Raw Data'!G354</f>
+        <v>0.35912014260390301</v>
       </c>
       <c r="H354">
         <v>0.30992375486624402</v>
@@ -27764,7 +27768,11 @@
       </c>
       <c r="F355">
         <f>'CPP Raw Data'!F355*-1</f>
-        <v>0.29925972432418002</v>
+        <v>0.29955444122375902</v>
+      </c>
+      <c r="G355">
+        <f>'CPP Raw Data'!G355</f>
+        <v>0.28249040717322799</v>
       </c>
       <c r="H355">
         <v>0.21505382645528601</v>
@@ -27801,7 +27809,11 @@
       </c>
       <c r="F356">
         <f>'CPP Raw Data'!F356*-1</f>
-        <v>0.30950482242639998</v>
+        <v>0.295221227647949</v>
+      </c>
+      <c r="G356">
+        <f>'CPP Raw Data'!G356</f>
+        <v>0.27797020214826601</v>
       </c>
       <c r="H356">
         <v>0.264864983542688</v>
@@ -27838,7 +27850,11 @@
       </c>
       <c r="F357">
         <f>'CPP Raw Data'!F357*-1</f>
-        <v>0.13446084827725799</v>
+        <v>9.2509318242914404E-2</v>
+      </c>
+      <c r="G357">
+        <f>'CPP Raw Data'!G357</f>
+        <v>0.185452620434893</v>
       </c>
       <c r="H357">
         <v>0.100093821264926</v>
@@ -27875,7 +27891,11 @@
       </c>
       <c r="F358">
         <f>'CPP Raw Data'!F358*-1</f>
-        <v>0.27801245180987999</v>
+        <v>0.26415360555396999</v>
+      </c>
+      <c r="G358">
+        <f>'CPP Raw Data'!G358</f>
+        <v>0.27685857902939298</v>
       </c>
       <c r="H358">
         <v>0.228909325864326</v>
@@ -27912,7 +27932,11 @@
       </c>
       <c r="F359">
         <f>'CPP Raw Data'!F359*-1</f>
-        <v>0.219360366827901</v>
+        <v>0.184083803393538</v>
+      </c>
+      <c r="G359">
+        <f>'CPP Raw Data'!G359</f>
+        <v>0.21435982928137601</v>
       </c>
       <c r="H359">
         <v>0.18596083621951301</v>
@@ -27949,7 +27973,11 @@
       </c>
       <c r="F360">
         <f>'CPP Raw Data'!F360*-1</f>
-        <v>0.317768205323473</v>
+        <v>0.32524018090110501</v>
+      </c>
+      <c r="G360">
+        <f>'CPP Raw Data'!G360</f>
+        <v>0.35250381827727201</v>
       </c>
       <c r="H360">
         <v>0.28326514132664798</v>
@@ -27986,7 +28014,11 @@
       </c>
       <c r="F361">
         <f>'CPP Raw Data'!F361*-1</f>
-        <v>0.28219456040659802</v>
+        <v>0.28841451924082401</v>
+      </c>
+      <c r="G361">
+        <f>'CPP Raw Data'!G361</f>
+        <v>0.27989431265986497</v>
       </c>
       <c r="H361">
         <v>0.24026804793939099</v>
@@ -28023,7 +28055,11 @@
       </c>
       <c r="F362">
         <f>'CPP Raw Data'!F362*-1</f>
-        <v>0.35442831584472101</v>
+        <v>0.36471099338607998</v>
+      </c>
+      <c r="G362">
+        <f>'CPP Raw Data'!G362</f>
+        <v>0.30940835284337398</v>
       </c>
       <c r="H362">
         <v>0.361291002672605</v>
@@ -28060,7 +28096,11 @@
       </c>
       <c r="F363">
         <f>'CPP Raw Data'!F363*-1</f>
-        <v>0.21488559731531001</v>
+        <v>0.220912708265362</v>
+      </c>
+      <c r="G363">
+        <f>'CPP Raw Data'!G363</f>
+        <v>0.21666368504615699</v>
       </c>
       <c r="H363">
         <v>0.18985524961846101</v>
@@ -28097,7 +28137,11 @@
       </c>
       <c r="F364">
         <f>'CPP Raw Data'!F364*-1</f>
-        <v>0.41520452595749502</v>
+        <v>0.42629961971025099</v>
+      </c>
+      <c r="G364">
+        <f>'CPP Raw Data'!G364</f>
+        <v>0.36876337056372299</v>
       </c>
       <c r="H364">
         <v>0.35361934361397901</v>
@@ -28134,7 +28178,11 @@
       </c>
       <c r="F365">
         <f>'CPP Raw Data'!F365*-1</f>
-        <v>0.447733667546654</v>
+        <v>0.44362779776128702</v>
+      </c>
+      <c r="G365">
+        <f>'CPP Raw Data'!G365</f>
+        <v>0.42681421208526199</v>
       </c>
       <c r="H365">
         <v>0.35409365521675101</v>
@@ -28171,7 +28219,11 @@
       </c>
       <c r="F366">
         <f>'CPP Raw Data'!F366*-1</f>
-        <v>8.3436357848605702E-2</v>
+        <v>0.12666836272446799</v>
+      </c>
+      <c r="G366">
+        <f>'CPP Raw Data'!G366</f>
+        <v>-7.4013722657988402E-3</v>
       </c>
       <c r="H366">
         <v>1.34358691830649E-2</v>
@@ -28208,7 +28260,11 @@
       </c>
       <c r="F367">
         <f>'CPP Raw Data'!F367*-1</f>
-        <v>0.273195091470605</v>
+        <v>0.26253497248445401</v>
+      </c>
+      <c r="G367">
+        <f>'CPP Raw Data'!G367</f>
+        <v>0.23537657142616</v>
       </c>
       <c r="H367">
         <v>0.225086414463185</v>
@@ -28245,7 +28301,11 @@
       </c>
       <c r="F368">
         <f>'CPP Raw Data'!F368*-1</f>
-        <v>0.36429992932970701</v>
+        <v>0.360250685937689</v>
+      </c>
+      <c r="G368">
+        <f>'CPP Raw Data'!G368</f>
+        <v>0.31084185247051699</v>
       </c>
       <c r="H368">
         <v>0.30278271789310202</v>
@@ -28282,7 +28342,11 @@
       </c>
       <c r="F369">
         <f>'CPP Raw Data'!F369*-1</f>
-        <v>0.26029880418155199</v>
+        <v>0.24869400738938199</v>
+      </c>
+      <c r="G369">
+        <f>'CPP Raw Data'!G369</f>
+        <v>0.29444849354054298</v>
       </c>
       <c r="H369">
         <v>0.20962491980534301</v>
@@ -28319,7 +28383,11 @@
       </c>
       <c r="F370">
         <f>'CPP Raw Data'!F370*-1</f>
-        <v>0.23214390399518001</v>
+        <v>0.20602717489400699</v>
+      </c>
+      <c r="G370">
+        <f>'CPP Raw Data'!G370</f>
+        <v>0.252844112094046</v>
       </c>
       <c r="H370">
         <v>0.19779819010084099</v>
@@ -28356,7 +28424,11 @@
       </c>
       <c r="F371">
         <f>'CPP Raw Data'!F371*-1</f>
-        <v>0.36830687069829199</v>
+        <v>0.34810302328603998</v>
+      </c>
+      <c r="G371">
+        <f>'CPP Raw Data'!G371</f>
+        <v>0.379587030488933</v>
       </c>
       <c r="H371">
         <v>0.249663650635741</v>
@@ -28393,7 +28465,11 @@
       </c>
       <c r="F372">
         <f>'CPP Raw Data'!F372*-1</f>
-        <v>0.29743949915703</v>
+        <v>0.28291035621155902</v>
+      </c>
+      <c r="G372">
+        <f>'CPP Raw Data'!G372</f>
+        <v>0.28249109288871699</v>
       </c>
       <c r="H372">
         <v>0.216916341198305</v>
@@ -28430,7 +28506,11 @@
       </c>
       <c r="F373">
         <f>'CPP Raw Data'!F373*-1</f>
-        <v>0.164961891908988</v>
+        <v>0.173097165610094</v>
+      </c>
+      <c r="G373">
+        <f>'CPP Raw Data'!G373</f>
+        <v>0.114605321491316</v>
       </c>
       <c r="H373">
         <v>0.12284799293635899</v>
@@ -28467,7 +28547,11 @@
       </c>
       <c r="F374">
         <f>'CPP Raw Data'!F374*-1</f>
-        <v>0.30139383892994698</v>
+        <v>0.29541091967112898</v>
+      </c>
+      <c r="G374">
+        <f>'CPP Raw Data'!G374</f>
+        <v>0.30826536441119001</v>
       </c>
       <c r="H374">
         <v>0.26571388283234898</v>
@@ -28504,7 +28588,11 @@
       </c>
       <c r="F375">
         <f>'CPP Raw Data'!F375*-1</f>
-        <v>0.228907627418419</v>
+        <v>0.22431720718596901</v>
+      </c>
+      <c r="G375">
+        <f>'CPP Raw Data'!G375</f>
+        <v>0.21057970350080901</v>
       </c>
       <c r="H375">
         <v>0.17938985047494799</v>
@@ -28541,7 +28629,11 @@
       </c>
       <c r="F376">
         <f>'CPP Raw Data'!F376*-1</f>
-        <v>1.24343151543838E-3</v>
+        <v>3.3107523834437803E-2</v>
+      </c>
+      <c r="G376">
+        <f>'CPP Raw Data'!G376</f>
+        <v>-4.0350439421496E-2</v>
       </c>
       <c r="H376">
         <v>0.100620567375887</v>
@@ -28578,7 +28670,11 @@
       </c>
       <c r="F377">
         <f>'CPP Raw Data'!F377*-1</f>
-        <v>0.283737323718741</v>
+        <v>0.27979642897650903</v>
+      </c>
+      <c r="G377">
+        <f>'CPP Raw Data'!G377</f>
+        <v>0.25781723239297499</v>
       </c>
       <c r="H377">
         <v>0.181012204688411</v>
@@ -28615,7 +28711,11 @@
       </c>
       <c r="F378">
         <f>'CPP Raw Data'!F378*-1</f>
-        <v>0.36634556095582299</v>
+        <v>0.351878315555814</v>
+      </c>
+      <c r="G378">
+        <f>'CPP Raw Data'!G378</f>
+        <v>0.34204337718320199</v>
       </c>
       <c r="H378">
         <v>0.31973733331240201</v>
@@ -28652,7 +28752,11 @@
       </c>
       <c r="F379">
         <f>'CPP Raw Data'!F379*-1</f>
-        <v>0.23917940716426001</v>
+        <v>0.240250090861824</v>
+      </c>
+      <c r="G379">
+        <f>'CPP Raw Data'!G379</f>
+        <v>0.24211507885615199</v>
       </c>
       <c r="H379">
         <v>0.200213872227641</v>
@@ -28689,7 +28793,11 @@
       </c>
       <c r="F380">
         <f>'CPP Raw Data'!F380*-1</f>
-        <v>0.102301192284214</v>
+        <v>8.9747743397998098E-2</v>
+      </c>
+      <c r="G380">
+        <f>'CPP Raw Data'!G380</f>
+        <v>4.9754148226134602E-2</v>
       </c>
       <c r="H380">
         <v>3.27839920369635E-2</v>
@@ -28726,7 +28834,11 @@
       </c>
       <c r="F381">
         <f>'CPP Raw Data'!F381*-1</f>
-        <v>0.33383374127676602</v>
+        <v>0.313448515722691</v>
+      </c>
+      <c r="G381">
+        <f>'CPP Raw Data'!G381</f>
+        <v>0.29730749235929099</v>
       </c>
       <c r="H381">
         <v>0.277880377721761</v>
@@ -28763,7 +28875,11 @@
       </c>
       <c r="F382">
         <f>'CPP Raw Data'!F382*-1</f>
-        <v>0.26819872912488302</v>
+        <v>0.26224751643500699</v>
+      </c>
+      <c r="G382">
+        <f>'CPP Raw Data'!G382</f>
+        <v>0.252823852647378</v>
       </c>
       <c r="H382">
         <v>0.20246532880072701</v>
@@ -28800,7 +28916,11 @@
       </c>
       <c r="F383">
         <f>'CPP Raw Data'!F383*-1</f>
-        <v>0.36425547484376702</v>
+        <v>0.37005442936209798</v>
+      </c>
+      <c r="G383">
+        <f>'CPP Raw Data'!G383</f>
+        <v>0.35799053992732299</v>
       </c>
       <c r="H383">
         <v>0.32919268948908498</v>
@@ -28837,7 +28957,11 @@
       </c>
       <c r="F384">
         <f>'CPP Raw Data'!F384*-1</f>
-        <v>0.23233304076366301</v>
+        <v>0.227420721545668</v>
+      </c>
+      <c r="G384">
+        <f>'CPP Raw Data'!G384</f>
+        <v>0.20680585391822301</v>
       </c>
       <c r="H384">
         <v>0.18386422850376799</v>
@@ -28874,7 +28998,11 @@
       </c>
       <c r="F385">
         <f>'CPP Raw Data'!F385*-1</f>
-        <v>0.28547293427922299</v>
+        <v>0.27646412232504097</v>
+      </c>
+      <c r="G385">
+        <f>'CPP Raw Data'!G385</f>
+        <v>0.261331118780046</v>
       </c>
       <c r="H385">
         <v>0.206553339452343</v>
@@ -28901,8 +29029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29231,7 +29359,11 @@
       </c>
       <c r="C13">
         <f>AVERAGEIF('Flipped data - to use'!$B$2:$B$385,'Scotland Data - use'!$A13,'Flipped data - to use'!F$2:F$385)</f>
-        <v>0.27173000922019708</v>
+        <v>0.26688757424928422</v>
+      </c>
+      <c r="D13">
+        <f>AVERAGEIF('Flipped data - to use'!$B$2:$B$385,'Scotland Data - use'!$A13,'Flipped data - to use'!G$2:G$385)</f>
+        <v>0.2549867486581992</v>
       </c>
       <c r="E13">
         <f>AVERAGEIF('Flipped data - to use'!$B$2:$B$385,'Scotland Data - use'!$A13,'Flipped data - to use'!H$2:H$385)</f>
@@ -29256,6 +29388,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010081FAC630D54E9140B4AB806285961C20" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4b1ff426f6ab44433fa90133b41c6530">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0ffb6a14-689f-42ef-a067-675c51ff5d7a" xmlns:ns4="a011b53f-306d-4901-9018-6d427f6237fb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="945afaefde5cbe62288d729dbeb08812" ns3:_="" ns4:_="">
     <xsd:import namespace="0ffb6a14-689f-42ef-a067-675c51ff5d7a"/>
@@ -29472,12 +29610,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -29488,6 +29620,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{082F13FD-C70D-418E-A1E2-3A104DB84F0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E040864-2A97-4C78-85E7-DAE01F518143}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -29506,15 +29647,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{082F13FD-C70D-418E-A1E2-3A104DB84F0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D13426F8-84C3-46C1-A03F-03F10DAB276F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fix error in Duncan Index data
</commit_message>
<xml_diff>
--- a/Duncan_Index/Duncan index by FINALAUG22.xlsx
+++ b/Duncan_Index/Duncan index by FINALAUG22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://impservihub-my.sharepoint.com/personal/nicholas_cassidy_improvementservice_org_uk/Documents/CPOP/Duncan_Index/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="8_{9A9C2946-D7BA-4757-8564-DD044F70F428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC1ED892-4958-4AEC-B76B-5E84C551427E}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{9A9C2946-D7BA-4757-8564-DD044F70F428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F9FFF67-AC45-438D-97BA-16AE6C2DEA3C}"/>
   <bookViews>
-    <workbookView xWindow="3150" yWindow="3255" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="2" r:id="rId1"/>
@@ -29030,7 +29030,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H3" sqref="H3:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29091,6 +29091,10 @@
         <f>AVERAGEIF('Flipped data - to use'!$B$2:$B$385,'Scotland Data - use'!$A3,'Flipped data - to use'!J$2:J$385)</f>
         <v>-6.0226748907187364E-2</v>
       </c>
+      <c r="H3">
+        <f>AVERAGEIF('Flipped data - to use'!$B$2:$B$385,'Scotland Data - use'!$A3,'Flipped data - to use'!K$2:K$385)</f>
+        <v>0.24037129944889232</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -29107,6 +29111,10 @@
       <c r="G4">
         <f>AVERAGEIF('Flipped data - to use'!$B$2:$B$385,'Scotland Data - use'!$A4,'Flipped data - to use'!J$2:J$385)</f>
         <v>-5.7999851127981207E-2</v>
+      </c>
+      <c r="H4">
+        <f>AVERAGEIF('Flipped data - to use'!$B$2:$B$385,'Scotland Data - use'!$A4,'Flipped data - to use'!K$2:K$385)</f>
+        <v>0.23691914230015471</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -29388,9 +29396,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29611,19 +29622,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{082F13FD-C70D-418E-A1E2-3A104DB84F0D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D13426F8-84C3-46C1-A03F-03F10DAB276F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -29648,9 +29655,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D13426F8-84C3-46C1-A03F-03F10DAB276F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{082F13FD-C70D-418E-A1E2-3A104DB84F0D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>